<commit_message>
求职招聘先隐藏 const showJobFlag = false;
</commit_message>
<xml_diff>
--- a/isoft_doc/工作安排.xlsx
+++ b/isoft_doc/工作安排.xlsx
@@ -14,14 +14,14 @@
     <sheet name="未来规划" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">能力统计!$A$1:$F$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">能力统计!$A$1:$F$118</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="194">
   <si>
     <t>模块</t>
   </si>
@@ -301,6 +301,9 @@
     <t>页面排版优化</t>
   </si>
   <si>
+    <t>博客、书单、课程</t>
+  </si>
+  <si>
     <t>1.VIP特权图标：①招聘的时候"荐" ②头像icon上加一个帽子
 文案修改、VIP价格修改：12/30/50/80</t>
   </si>
@@ -364,9 +367,15 @@
     <t>消息模块</t>
   </si>
   <si>
+    <t>接下来重点</t>
+  </si>
+  <si>
     <t>发现</t>
   </si>
   <si>
+    <t>再具体设计一些方案</t>
+  </si>
+  <si>
     <t>我要赚钱</t>
   </si>
   <si>
@@ -409,6 +418,15 @@
     <t>控制台</t>
   </si>
   <si>
+    <t>风险控制-&gt;文件上传监控（fileupload_log表添加文件大小字段：file_size）</t>
+  </si>
+  <si>
+    <t>自己摸索下</t>
+  </si>
+  <si>
+    <t>把用户查询功能做出来</t>
+  </si>
+  <si>
     <t>所有模块</t>
   </si>
   <si>
@@ -431,6 +449,9 @@
   </si>
   <si>
     <t>链知首页图片优化</t>
+  </si>
+  <si>
+    <t>考虑添加悬赏功能</t>
   </si>
   <si>
     <t>准备订单模块的策划和编写</t>
@@ -455,10 +476,16 @@
     <t>求问专家里面的用户印象标签可以复用到其他模块。</t>
   </si>
   <si>
+    <t>复制成功，提示修改</t>
+  </si>
+  <si>
     <t>路由需要优化为单词，去掉下划线</t>
   </si>
   <si>
     <t>VoteTags引用到各个模块</t>
+  </si>
+  <si>
+    <t>网站各个地方多加动画</t>
   </si>
   <si>
     <t>图片按照模块来划分，每个模块一个文件夹</t>
@@ -719,10 +746,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -742,28 +769,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -771,37 +776,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -830,6 +812,82 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -847,37 +905,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -917,7 +944,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -929,55 +1112,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -989,115 +1124,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1111,11 +1138,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1153,47 +1219,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1216,10 +1243,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1228,16 +1255,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1246,115 +1273,115 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1773,16 +1800,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F113"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="20.3636363636364" style="3" customWidth="1"/>
-    <col min="2" max="2" width="63.7272727272727" style="3" customWidth="1"/>
+    <col min="2" max="2" width="70.6363636363636" style="3" customWidth="1"/>
     <col min="3" max="3" width="47.2727272727273" style="3" customWidth="1"/>
     <col min="4" max="4" width="22.6363636363636" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.0909090909091" style="3" customWidth="1"/>
@@ -2466,12 +2493,15 @@
       <c r="B64" s="17" t="s">
         <v>86</v>
       </c>
+      <c r="C64" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="D64" s="6"/>
       <c r="E64" s="7"/>
     </row>
     <row r="65" ht="28" spans="2:5">
       <c r="B65" s="14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D65" s="6">
         <v>43940</v>
@@ -2482,7 +2512,7 @@
     </row>
     <row r="66" ht="28" spans="2:5">
       <c r="B66" s="16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D66" s="6">
         <v>43893</v>
@@ -2493,10 +2523,10 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D67" s="6">
         <v>43939</v>
@@ -2507,7 +2537,7 @@
     </row>
     <row r="68" spans="2:5">
       <c r="B68" s="15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D68" s="6">
         <v>43940</v>
@@ -2518,10 +2548,10 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D69" s="6">
         <v>43873</v>
@@ -2532,7 +2562,7 @@
     </row>
     <row r="70" spans="2:5">
       <c r="B70" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D70" s="6">
         <v>43873</v>
@@ -2543,7 +2573,7 @@
     </row>
     <row r="71" spans="2:5">
       <c r="B71" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D71" s="6">
         <v>43873</v>
@@ -2554,7 +2584,7 @@
     </row>
     <row r="72" spans="2:5">
       <c r="B72" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D72" s="6">
         <v>43873</v>
@@ -2565,7 +2595,7 @@
     </row>
     <row r="73" spans="2:5">
       <c r="B73" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D73" s="6">
         <v>43940</v>
@@ -2576,7 +2606,7 @@
     </row>
     <row r="74" spans="2:5">
       <c r="B74" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D74" s="6">
         <v>43873</v>
@@ -2587,7 +2617,7 @@
     </row>
     <row r="75" spans="2:5">
       <c r="B75" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D75" s="6">
         <v>43873</v>
@@ -2598,7 +2628,7 @@
     </row>
     <row r="76" ht="42" spans="2:5">
       <c r="B76" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D76" s="6">
         <v>43873</v>
@@ -2609,7 +2639,7 @@
     </row>
     <row r="77" spans="2:5">
       <c r="B77" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D77" s="6">
         <v>43873</v>
@@ -2620,16 +2650,16 @@
     </row>
     <row r="78" spans="2:5">
       <c r="B78" s="16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E78" s="21"/>
     </row>
     <row r="79" spans="2:5">
       <c r="B79" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D79" s="6">
         <v>43904</v>
@@ -2640,7 +2670,7 @@
     </row>
     <row r="80" spans="2:5">
       <c r="B80" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D80" s="6">
         <v>43873</v>
@@ -2649,36 +2679,42 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:3">
       <c r="A81" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B81" s="17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
+        <v>104</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B84" s="17"/>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D85" s="6">
         <v>43868</v>
@@ -2689,41 +2725,41 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="2:2">
       <c r="B87" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B90" s="17" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D91" s="6">
         <v>43881</v>
@@ -2732,56 +2768,52 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:5">
       <c r="A92" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B93" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" s="5"/>
+        <v>124</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D92" s="6"/>
+      <c r="E92" s="7"/>
+    </row>
+    <row r="93" spans="4:5">
+      <c r="D93" s="6"/>
+      <c r="E93" s="7"/>
+    </row>
+    <row r="94" spans="2:3">
       <c r="B94" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
-      <c r="A95" s="5"/>
-      <c r="B95" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D95" s="6">
-        <v>43894</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
+        <v>127</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B95" s="17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
       <c r="A96" s="5"/>
-      <c r="B96" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="D96" s="6">
-        <v>43888</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>7</v>
+      <c r="B96" s="17" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="5"/>
-      <c r="B97" s="15" t="s">
-        <v>127</v>
+      <c r="B97" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="D97" s="6">
-        <v>43919</v>
+        <v>43894</v>
       </c>
       <c r="E97" s="7" t="s">
         <v>7</v>
@@ -2790,10 +2822,10 @@
     <row r="98" spans="1:5">
       <c r="A98" s="5"/>
       <c r="B98" s="15" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D98" s="6">
-        <v>43890</v>
+        <v>43888</v>
       </c>
       <c r="E98" s="7" t="s">
         <v>7</v>
@@ -2802,10 +2834,10 @@
     <row r="99" spans="1:5">
       <c r="A99" s="5"/>
       <c r="B99" s="15" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D99" s="6">
-        <v>43881</v>
+        <v>43919</v>
       </c>
       <c r="E99" s="7" t="s">
         <v>7</v>
@@ -2814,13 +2846,10 @@
     <row r="100" spans="1:5">
       <c r="A100" s="5"/>
       <c r="B100" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D100" s="6">
-        <v>43940</v>
+        <v>43890</v>
       </c>
       <c r="E100" s="7" t="s">
         <v>7</v>
@@ -2829,34 +2858,33 @@
     <row r="101" spans="1:5">
       <c r="A101" s="5"/>
       <c r="B101" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D101" s="6">
-        <v>43904</v>
+        <v>43881</v>
       </c>
       <c r="E101" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="102" ht="28" spans="1:3">
+    <row r="102" spans="1:5">
       <c r="A102" s="5"/>
-      <c r="B102" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="C102" s="17" t="s">
-        <v>135</v>
-      </c>
+      <c r="B102" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="D102" s="6"/>
+      <c r="E102" s="7"/>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="5"/>
-      <c r="B103" s="16" t="s">
-        <v>136</v>
+      <c r="B103" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="D103" s="6">
-        <v>43919</v>
+        <v>43940</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>7</v>
@@ -2865,7 +2893,10 @@
     <row r="104" spans="1:5">
       <c r="A104" s="5"/>
       <c r="B104" s="15" t="s">
-        <v>137</v>
+        <v>139</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="D104" s="6">
         <v>43904</v>
@@ -2874,71 +2905,121 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" ht="28" spans="1:3">
       <c r="A105" s="5"/>
-      <c r="B105" s="15" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
+      <c r="B105" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C105" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" s="5"/>
-      <c r="B106" s="17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
+      <c r="B106" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D106" s="6">
+        <v>43919</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" s="5"/>
-      <c r="B107" s="17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="108" ht="28" spans="1:2">
+      <c r="B107" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D107" s="6"/>
+      <c r="E107" s="7"/>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" s="5"/>
-      <c r="B108" s="16" t="s">
-        <v>141</v>
+      <c r="B108" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="D108" s="6">
+        <v>43904</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="5"/>
-      <c r="B109" s="18" t="s">
-        <v>142</v>
+      <c r="B109" s="15" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="5"/>
       <c r="B110" s="17" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="5"/>
       <c r="B111" s="15" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
       <c r="A112" s="5"/>
-      <c r="B112" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="D112" s="6">
-        <v>43940</v>
-      </c>
-      <c r="E112" s="7" t="s">
-        <v>7</v>
+      <c r="B112" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="113" ht="28" spans="1:2">
       <c r="A113" s="5"/>
-      <c r="B113" s="18" t="s">
-        <v>146</v>
+      <c r="B113" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="5"/>
+      <c r="B114" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="5"/>
+      <c r="B115" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="5"/>
+      <c r="B116" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="5"/>
+      <c r="B117" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D117" s="6">
+        <v>43940</v>
+      </c>
+      <c r="E117" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" ht="28" spans="1:2">
+      <c r="A118" s="5"/>
+      <c r="B118" s="18" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F113">
+  <autoFilter ref="A1:F118">
     <extLst/>
   </autoFilter>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A14"/>
     <mergeCell ref="A15:A39"/>
@@ -2950,7 +3031,8 @@
     <mergeCell ref="A67:A68"/>
     <mergeCell ref="A69:A80"/>
     <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A93:A113"/>
+    <mergeCell ref="A92:A94"/>
+    <mergeCell ref="A95:A118"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2980,16 +3062,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="9" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>3</v>
@@ -3000,16 +3082,16 @@
     </row>
     <row r="2" ht="49" customHeight="1" spans="1:6">
       <c r="A2" s="9" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="E2" s="6">
         <v>43867</v>
@@ -3020,16 +3102,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="9" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="E3" s="6">
         <v>43877</v>
@@ -3040,32 +3122,32 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="9" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="9" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="E5" s="6">
         <v>43877</v>
@@ -3076,16 +3158,16 @@
     </row>
     <row r="6" ht="37" customHeight="1" spans="1:6">
       <c r="A6" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>163</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>154</v>
       </c>
       <c r="E6" s="6">
         <v>43867</v>
@@ -3097,13 +3179,13 @@
     <row r="7" ht="48" customHeight="1" spans="1:6">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="E7" s="6">
         <v>43867</v>
@@ -3114,16 +3196,16 @@
     </row>
     <row r="8" ht="43" customHeight="1" spans="1:6">
       <c r="A8" s="9" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="E8" s="6">
         <v>43936</v>
@@ -3135,13 +3217,13 @@
     <row r="9" ht="37" customHeight="1" spans="1:6">
       <c r="A9" s="9"/>
       <c r="B9" s="11" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="E9" s="6">
         <v>43936</v>
@@ -3152,16 +3234,16 @@
     </row>
     <row r="10" ht="59" customHeight="1" spans="1:6">
       <c r="A10" s="9" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="E10" s="6">
         <v>43876</v>
@@ -3203,16 +3285,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -3223,16 +3305,16 @@
     </row>
     <row r="2" ht="42" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E2" s="6">
         <v>43867</v>
@@ -3243,16 +3325,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E3" s="6">
         <v>43877</v>
@@ -3263,32 +3345,32 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="7"/>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E5" s="6">
         <v>43877</v>
@@ -3299,16 +3381,16 @@
     </row>
     <row r="6" ht="48" customHeight="1" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E6" s="6">
         <v>43867</v>
@@ -3319,13 +3401,13 @@
     </row>
     <row r="7" ht="45" customHeight="1" spans="2:6">
       <c r="B7" s="3" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E7" s="6">
         <v>43867</v>
@@ -3336,16 +3418,16 @@
     </row>
     <row r="8" ht="44" customHeight="1" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E8" s="6">
         <v>43936</v>
@@ -3356,13 +3438,13 @@
     </row>
     <row r="9" ht="47" customHeight="1" spans="2:6">
       <c r="B9" s="5" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E9" s="6">
         <v>43936</v>
@@ -3373,16 +3455,16 @@
     </row>
     <row r="10" ht="48" customHeight="1" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="E10" s="6">
         <v>43876</v>
@@ -3421,22 +3503,22 @@
   <sheetData>
     <row r="1" ht="23" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" ht="56" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="1" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Author:z001 - Reason: App 需求规划]
</commit_message>
<xml_diff>
--- a/isoft_doc/工作安排.xlsx
+++ b/isoft_doc/工作安排.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="223">
   <si>
     <t>模块</t>
   </si>
@@ -545,10 +545,61 @@
 未登录状态，逐个测试</t>
   </si>
   <si>
+    <t>开屏广告页</t>
+  </si>
+  <si>
     <t>首页</t>
   </si>
   <si>
-    <t>课程</t>
+    <t>首页侧边栏分类</t>
+  </si>
+  <si>
+    <t>空间-我的收藏</t>
+  </si>
+  <si>
+    <t>空间-观看记录</t>
+  </si>
+  <si>
+    <t>空间-订单信息</t>
+  </si>
+  <si>
+    <t>登录注册页面</t>
+  </si>
+  <si>
+    <t>课程详情页面</t>
+  </si>
+  <si>
+    <t>课程详情展示</t>
+  </si>
+  <si>
+    <t>课程收藏、点赞功能展示</t>
+  </si>
+  <si>
+    <t>评论列表展示、删除等功能</t>
+  </si>
+  <si>
+    <t>课程播放页面</t>
+  </si>
+  <si>
+    <t>课程分类页面</t>
+  </si>
+  <si>
+    <t>查看全部分类</t>
+  </si>
+  <si>
+    <t>查看推荐分类（java、前端、后端、基础等）</t>
+  </si>
+  <si>
+    <t>课程推荐页面</t>
+  </si>
+  <si>
+    <t>课程搜索页面</t>
+  </si>
+  <si>
+    <t>功能列表页面</t>
+  </si>
+  <si>
+    <t>活动、商业合作、名师招募等</t>
   </si>
   <si>
     <t>配置项</t>
@@ -793,9 +844,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -822,30 +873,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -859,17 +889,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -898,7 +919,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -909,6 +938,36 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -929,23 +988,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -997,13 +1048,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1015,7 +1090,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1027,19 +1150,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1051,43 +1204,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1099,79 +1216,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1187,24 +1238,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1234,6 +1272,39 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -1244,26 +1315,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1290,149 +1341,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1475,11 +1526,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1852,8 +1906,8 @@
   <sheetPr/>
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1862,7 +1916,7 @@
     <col min="2" max="2" width="70.6363636363636" style="5" customWidth="1"/>
     <col min="3" max="3" width="47.2727272727273" style="5" customWidth="1"/>
     <col min="4" max="4" width="22.6363636363636" style="5" customWidth="1"/>
-    <col min="5" max="5" width="4.27272727272727" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.0909090909091" style="5" customWidth="1"/>
     <col min="6" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
@@ -1934,7 +1988,7 @@
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1970,7 +2024,7 @@
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="8"/>
@@ -2002,7 +2056,7 @@
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="8">
@@ -2059,7 +2113,7 @@
       </c>
     </row>
     <row r="18" spans="2:2">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="17" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2123,7 +2177,7 @@
       </c>
     </row>
     <row r="26" ht="42" spans="2:5">
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="18" t="s">
         <v>35</v>
       </c>
       <c r="D26" s="8">
@@ -2134,10 +2188,10 @@
       </c>
     </row>
     <row r="27" ht="28" spans="2:5">
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="19" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="8">
@@ -2153,7 +2207,7 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="17" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="8">
@@ -2186,10 +2240,10 @@
       </c>
     </row>
     <row r="32" ht="56" spans="2:5">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="19" t="s">
         <v>43</v>
       </c>
       <c r="D32" s="8">
@@ -2233,7 +2287,7 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="17" t="s">
         <v>47</v>
       </c>
       <c r="D36" s="8">
@@ -2244,7 +2298,7 @@
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="18" t="s">
         <v>48</v>
       </c>
       <c r="D37" s="8">
@@ -2255,7 +2309,7 @@
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="18" t="s">
         <v>49</v>
       </c>
       <c r="D38" s="8">
@@ -2266,7 +2320,7 @@
       </c>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="18" t="s">
         <v>50</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -2316,7 +2370,7 @@
       </c>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="17" t="s">
         <v>56</v>
       </c>
       <c r="D43" s="8">
@@ -2327,10 +2381,10 @@
       </c>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="15"/>
+      <c r="C44" s="17"/>
       <c r="D44" s="8">
         <v>43896</v>
       </c>
@@ -2350,7 +2404,7 @@
       </c>
     </row>
     <row r="46" spans="2:5">
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="17" t="s">
         <v>59</v>
       </c>
       <c r="C46" s="5" t="s">
@@ -2395,10 +2449,10 @@
       <c r="E49" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F49" s="15"/>
+      <c r="F49" s="17"/>
     </row>
     <row r="50" spans="2:6">
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="17" t="s">
         <v>64</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -2410,10 +2464,10 @@
       <c r="E50" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F50" s="15"/>
+      <c r="F50" s="17"/>
     </row>
     <row r="51" spans="2:6">
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="17" t="s">
         <v>66</v>
       </c>
       <c r="C51" s="5" t="s">
@@ -2425,7 +2479,7 @@
       <c r="E51" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F51" s="15"/>
+      <c r="F51" s="17"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="5" t="s">
@@ -2442,10 +2496,10 @@
       <c r="A53" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="21" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2458,7 +2512,7 @@
       <c r="A55" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="17" t="s">
         <v>73</v>
       </c>
       <c r="D55" s="8">
@@ -2469,15 +2523,15 @@
       </c>
     </row>
     <row r="56" spans="2:3">
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C56" s="20" t="s">
+      <c r="C56" s="21" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="57" ht="28" spans="2:3">
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="18" t="s">
         <v>75</v>
       </c>
       <c r="C57" s="5" t="s">
@@ -2485,7 +2539,7 @@
       </c>
     </row>
     <row r="58" spans="2:3">
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="18" t="s">
         <v>77</v>
       </c>
       <c r="C58" s="5" t="s">
@@ -2493,7 +2547,7 @@
       </c>
     </row>
     <row r="59" spans="2:5">
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="17" t="s">
         <v>79</v>
       </c>
       <c r="D59" s="8">
@@ -2507,7 +2561,7 @@
       <c r="A60" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="17" t="s">
         <v>74</v>
       </c>
       <c r="D60" s="8">
@@ -2518,10 +2572,10 @@
       </c>
     </row>
     <row r="61" spans="2:4">
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D61" s="15"/>
+      <c r="D61" s="17"/>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="5" t="s">
@@ -2546,7 +2600,7 @@
       </c>
     </row>
     <row r="64" spans="2:5">
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="17" t="s">
         <v>86</v>
       </c>
       <c r="D64" s="8">
@@ -2557,7 +2611,7 @@
       </c>
     </row>
     <row r="65" spans="2:5">
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="17" t="s">
         <v>87</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -2571,7 +2625,7 @@
       </c>
     </row>
     <row r="66" ht="28" spans="2:5">
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="16" t="s">
         <v>89</v>
       </c>
       <c r="D66" s="8">
@@ -2582,7 +2636,7 @@
       </c>
     </row>
     <row r="67" ht="28" spans="2:5">
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="18" t="s">
         <v>90</v>
       </c>
       <c r="D67" s="8">
@@ -2596,7 +2650,7 @@
       <c r="A68" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B68" s="15" t="s">
+      <c r="B68" s="17" t="s">
         <v>92</v>
       </c>
       <c r="D68" s="8">
@@ -2607,7 +2661,7 @@
       </c>
     </row>
     <row r="69" spans="2:5">
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="17" t="s">
         <v>93</v>
       </c>
       <c r="D69" s="8">
@@ -2665,7 +2719,7 @@
       </c>
     </row>
     <row r="74" spans="2:5">
-      <c r="B74" s="15" t="s">
+      <c r="B74" s="17" t="s">
         <v>99</v>
       </c>
       <c r="D74" s="8">
@@ -2720,16 +2774,16 @@
       </c>
     </row>
     <row r="79" spans="2:5">
-      <c r="B79" s="17" t="s">
+      <c r="B79" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D79" s="21" t="s">
+      <c r="D79" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="E79" s="21"/>
+      <c r="E79" s="22"/>
     </row>
     <row r="80" spans="2:5">
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="18" t="s">
         <v>106</v>
       </c>
       <c r="D80" s="8">
@@ -2754,10 +2808,10 @@
       <c r="A82" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="B82" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="C82" s="18" t="s">
+      <c r="C82" s="19" t="s">
         <v>110</v>
       </c>
       <c r="D82" s="8">
@@ -2771,7 +2825,7 @@
       <c r="A83" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B83" s="18" t="s">
+      <c r="B83" s="19" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2784,7 +2838,7 @@
       <c r="A85" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B85" s="18"/>
+      <c r="B85" s="19"/>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="5" t="s">
@@ -2827,10 +2881,10 @@
       <c r="A91" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B91" s="18" t="s">
+      <c r="B91" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="C91" s="18" t="s">
+      <c r="C91" s="19" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2852,7 +2906,7 @@
       <c r="A93" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B93" s="18" t="s">
+      <c r="B93" s="19" t="s">
         <v>128</v>
       </c>
       <c r="C93" s="5" t="s">
@@ -2866,7 +2920,7 @@
       <c r="E94" s="9"/>
     </row>
     <row r="95" spans="2:5">
-      <c r="B95" s="15" t="s">
+      <c r="B95" s="17" t="s">
         <v>130</v>
       </c>
       <c r="C95" s="5" t="s">
@@ -2883,13 +2937,13 @@
       <c r="A96" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B96" s="18" t="s">
+      <c r="B96" s="19" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="7"/>
-      <c r="B97" s="15" t="s">
+      <c r="B97" s="17" t="s">
         <v>134</v>
       </c>
       <c r="C97" s="5" t="s">
@@ -2916,7 +2970,7 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="7"/>
-      <c r="B99" s="15" t="s">
+      <c r="B99" s="17" t="s">
         <v>137</v>
       </c>
       <c r="D99" s="8">
@@ -2928,7 +2982,7 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="7"/>
-      <c r="B100" s="15" t="s">
+      <c r="B100" s="17" t="s">
         <v>138</v>
       </c>
       <c r="D100" s="8">
@@ -2940,7 +2994,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="7"/>
-      <c r="B101" s="15" t="s">
+      <c r="B101" s="17" t="s">
         <v>139</v>
       </c>
       <c r="D101" s="8">
@@ -2952,7 +3006,7 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="7"/>
-      <c r="B102" s="15" t="s">
+      <c r="B102" s="17" t="s">
         <v>140</v>
       </c>
       <c r="D102" s="8">
@@ -2964,10 +3018,10 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="7"/>
-      <c r="B103" s="18" t="s">
+      <c r="B103" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="C103" s="18" t="s">
+      <c r="C103" s="19" t="s">
         <v>142</v>
       </c>
       <c r="D103" s="8"/>
@@ -2975,7 +3029,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="7"/>
-      <c r="B104" s="15" t="s">
+      <c r="B104" s="17" t="s">
         <v>143</v>
       </c>
       <c r="C104" s="5" t="s">
@@ -2990,7 +3044,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="7"/>
-      <c r="B105" s="15" t="s">
+      <c r="B105" s="17" t="s">
         <v>145</v>
       </c>
       <c r="C105" s="5" t="s">
@@ -3005,16 +3059,16 @@
     </row>
     <row r="106" ht="28" spans="1:3">
       <c r="A106" s="7"/>
-      <c r="B106" s="17" t="s">
+      <c r="B106" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="C106" s="18" t="s">
+      <c r="C106" s="19" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="7"/>
-      <c r="B107" s="17" t="s">
+      <c r="B107" s="18" t="s">
         <v>149</v>
       </c>
       <c r="D107" s="8">
@@ -3026,13 +3080,13 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="7"/>
-      <c r="B108" s="22" t="s">
+      <c r="B108" s="23" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="7"/>
-      <c r="B109" s="15" t="s">
+      <c r="B109" s="17" t="s">
         <v>151</v>
       </c>
       <c r="D109" s="8">
@@ -3044,28 +3098,28 @@
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="7"/>
-      <c r="B110" s="15" t="s">
+      <c r="B110" s="17" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="7"/>
-      <c r="B111" s="15" t="s">
+      <c r="B111" s="17" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="7"/>
-      <c r="B112" s="15" t="s">
+      <c r="B112" s="17" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="7"/>
-      <c r="B113" s="16" t="s">
+      <c r="B113" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="C113" s="16" t="s">
+      <c r="C113" s="17" t="s">
         <v>124</v>
       </c>
       <c r="D113" s="8">
@@ -3077,7 +3131,7 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="7"/>
-      <c r="B114" s="15" t="s">
+      <c r="B114" s="17" t="s">
         <v>156</v>
       </c>
       <c r="C114" s="5" t="s">
@@ -3086,13 +3140,13 @@
     </row>
     <row r="115" ht="28" spans="1:2">
       <c r="A115" s="7"/>
-      <c r="B115" s="17" t="s">
+      <c r="B115" s="18" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="7"/>
-      <c r="B116" s="17" t="s">
+      <c r="B116" s="18" t="s">
         <v>158</v>
       </c>
       <c r="D116" s="8">
@@ -3104,7 +3158,7 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="7"/>
-      <c r="B117" s="15" t="s">
+      <c r="B117" s="17" t="s">
         <v>159</v>
       </c>
       <c r="D117" s="8">
@@ -3116,7 +3170,7 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="7"/>
-      <c r="B118" s="15" t="s">
+      <c r="B118" s="17" t="s">
         <v>160</v>
       </c>
       <c r="D118" s="8">
@@ -3128,7 +3182,7 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="7"/>
-      <c r="B119" s="18" t="s">
+      <c r="B119" s="19" t="s">
         <v>161</v>
       </c>
       <c r="D119" s="8"/>
@@ -3136,7 +3190,7 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="7"/>
-      <c r="B120" s="15" t="s">
+      <c r="B120" s="17" t="s">
         <v>162</v>
       </c>
       <c r="D120" s="8">
@@ -3148,7 +3202,7 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="7"/>
-      <c r="B121" s="16" t="s">
+      <c r="B121" s="17" t="s">
         <v>163</v>
       </c>
       <c r="D121" s="8">
@@ -3160,13 +3214,13 @@
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="7"/>
-      <c r="B122" s="18" t="s">
+      <c r="B122" s="19" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="123" ht="28" spans="1:5">
       <c r="A123" s="7"/>
-      <c r="B123" s="17" t="s">
+      <c r="B123" s="18" t="s">
         <v>165</v>
       </c>
       <c r="D123" s="8">
@@ -3204,16 +3258,40 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="29.4545454545455" customWidth="1"/>
+    <col min="2" max="2" width="40.3636363636364" customWidth="1"/>
+    <col min="3" max="3" width="23.3636363636364" customWidth="1"/>
+    <col min="4" max="4" width="31.1818181818182" customWidth="1"/>
+    <col min="5" max="5" width="20.0909090909091" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>166</v>
       </c>
     </row>
@@ -3222,7 +3300,97 @@
         <v>167</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="14"/>
+      <c r="B5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="14"/>
+      <c r="B6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="14"/>
+      <c r="B9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="14"/>
+      <c r="B10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="14"/>
+      <c r="B13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="15"/>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" t="s">
+        <v>184</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A12:A14"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -3250,16 +3418,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -3270,16 +3438,16 @@
     </row>
     <row r="2" ht="49" customHeight="1" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="E2" s="8">
         <v>43867</v>
@@ -3290,16 +3458,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="E3" s="8">
         <v>43877</v>
@@ -3310,32 +3478,32 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="E5" s="8">
         <v>43877</v>
@@ -3346,16 +3514,16 @@
     </row>
     <row r="6" ht="37" customHeight="1" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="E6" s="8">
         <v>43867</v>
@@ -3367,13 +3535,13 @@
     <row r="7" ht="48" customHeight="1" spans="1:6">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="E7" s="8">
         <v>43867</v>
@@ -3384,16 +3552,16 @@
     </row>
     <row r="8" ht="43" customHeight="1" spans="1:6">
       <c r="A8" s="4" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="E8" s="8">
         <v>43936</v>
@@ -3405,13 +3573,13 @@
     <row r="9" ht="37" customHeight="1" spans="1:6">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>175</v>
       </c>
       <c r="E9" s="8">
         <v>43936</v>
@@ -3422,16 +3590,16 @@
     </row>
     <row r="10" ht="59" customHeight="1" spans="1:6">
       <c r="A10" s="4" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="E10" s="8">
         <v>43876</v>
@@ -3473,16 +3641,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>3</v>
@@ -3493,16 +3661,16 @@
     </row>
     <row r="2" ht="42" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="E2" s="8">
         <v>43867</v>
@@ -3513,16 +3681,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="E3" s="8">
         <v>43877</v>
@@ -3533,32 +3701,32 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="E5" s="8">
         <v>43877</v>
@@ -3569,16 +3737,16 @@
     </row>
     <row r="6" ht="48" customHeight="1" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="E6" s="8">
         <v>43867</v>
@@ -3589,13 +3757,13 @@
     </row>
     <row r="7" ht="45" customHeight="1" spans="2:6">
       <c r="B7" s="5" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="E7" s="8">
         <v>43867</v>
@@ -3606,16 +3774,16 @@
     </row>
     <row r="8" ht="44" customHeight="1" spans="1:6">
       <c r="A8" s="5" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="E8" s="8">
         <v>43936</v>
@@ -3626,13 +3794,13 @@
     </row>
     <row r="9" ht="47" customHeight="1" spans="2:6">
       <c r="B9" s="7" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="E9" s="8">
         <v>43936</v>
@@ -3643,16 +3811,16 @@
     </row>
     <row r="10" ht="48" customHeight="1" spans="1:6">
       <c r="A10" s="5" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="E10" s="8">
         <v>43876</v>
@@ -3691,22 +3859,22 @@
   <sheetData>
     <row r="1" ht="23" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" ht="42" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" ht="121" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:1">

</xml_diff>

<commit_message>
[Author:z001 - Reason: 工作安排完善]
</commit_message>
<xml_diff>
--- a/isoft_doc/工作安排.xlsx
+++ b/isoft_doc/工作安排.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7140"/>
+    <workbookView windowWidth="19200" windowHeight="7140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="web能力统计" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="234">
   <si>
     <t>模块</t>
   </si>
@@ -572,6 +572,18 @@
     <t>登录注册页面</t>
   </si>
   <si>
+    <t>登录功能：目前仅支持邮箱登录</t>
+  </si>
+  <si>
+    <t>注册功能样式优化</t>
+  </si>
+  <si>
+    <t>忘记密码和修改密码等功能</t>
+  </si>
+  <si>
+    <t>401 状态码全局拦截</t>
+  </si>
+  <si>
     <t>课程详情页面</t>
   </si>
   <si>
@@ -606,6 +618,21 @@
   </si>
   <si>
     <t>活动、商业合作、名师招募等</t>
+  </si>
+  <si>
+    <t>个人中心页面</t>
+  </si>
+  <si>
+    <t>发布的课程、收藏的课程、观看的视频展示</t>
+  </si>
+  <si>
+    <t>用户头像、用户标签语修改</t>
+  </si>
+  <si>
+    <t>公共能力</t>
+  </si>
+  <si>
+    <t>分页方案优化</t>
   </si>
   <si>
     <t>配置项</t>
@@ -879,25 +906,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -941,10 +961,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -955,9 +975,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -966,6 +985,21 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -987,13 +1021,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -1001,7 +1028,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1048,103 +1075,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1162,19 +1099,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1186,13 +1135,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1204,7 +1165,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1228,7 +1189,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1239,6 +1266,80 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1265,80 +1366,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1347,10 +1374,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1362,13 +1389,13 @@
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1377,115 +1404,115 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1532,6 +1559,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1551,12 +1584,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1909,8 +1936,8 @@
   <sheetPr/>
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1991,7 +2018,7 @@
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -2027,7 +2054,7 @@
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="8"/>
@@ -2059,7 +2086,7 @@
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="17" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="8">
@@ -2116,7 +2143,7 @@
       </c>
     </row>
     <row r="18" spans="2:2">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="17" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2180,7 +2207,7 @@
       </c>
     </row>
     <row r="26" ht="42" spans="2:5">
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="18" t="s">
         <v>35</v>
       </c>
       <c r="D26" s="8">
@@ -2191,10 +2218,10 @@
       </c>
     </row>
     <row r="27" ht="28" spans="2:5">
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="19" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="8">
@@ -2210,7 +2237,7 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="17" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="8">
@@ -2243,10 +2270,10 @@
       </c>
     </row>
     <row r="32" ht="56" spans="2:5">
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="19" t="s">
         <v>43</v>
       </c>
       <c r="D32" s="8">
@@ -2290,7 +2317,7 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="17" t="s">
         <v>47</v>
       </c>
       <c r="D36" s="8">
@@ -2301,7 +2328,7 @@
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="18" t="s">
         <v>48</v>
       </c>
       <c r="D37" s="8">
@@ -2312,7 +2339,7 @@
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="18" t="s">
         <v>49</v>
       </c>
       <c r="D38" s="8">
@@ -2323,7 +2350,7 @@
       </c>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="18" t="s">
         <v>50</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -2373,7 +2400,7 @@
       </c>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="17" t="s">
         <v>56</v>
       </c>
       <c r="D43" s="8">
@@ -2384,10 +2411,10 @@
       </c>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="15"/>
+      <c r="C44" s="17"/>
       <c r="D44" s="8">
         <v>43896</v>
       </c>
@@ -2407,7 +2434,7 @@
       </c>
     </row>
     <row r="46" spans="2:5">
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="17" t="s">
         <v>59</v>
       </c>
       <c r="C46" s="5" t="s">
@@ -2452,10 +2479,10 @@
       <c r="E49" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F49" s="15"/>
+      <c r="F49" s="17"/>
     </row>
     <row r="50" spans="2:6">
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="17" t="s">
         <v>64</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -2467,10 +2494,10 @@
       <c r="E50" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F50" s="15"/>
+      <c r="F50" s="17"/>
     </row>
     <row r="51" spans="2:6">
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="17" t="s">
         <v>66</v>
       </c>
       <c r="C51" s="5" t="s">
@@ -2482,7 +2509,7 @@
       <c r="E51" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F51" s="15"/>
+      <c r="F51" s="17"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="5" t="s">
@@ -2499,10 +2526,10 @@
       <c r="A53" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="21" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2515,7 +2542,7 @@
       <c r="A55" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="17" t="s">
         <v>73</v>
       </c>
       <c r="D55" s="8">
@@ -2526,15 +2553,15 @@
       </c>
     </row>
     <row r="56" spans="2:3">
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C56" s="21" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="57" ht="28" spans="2:3">
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="18" t="s">
         <v>75</v>
       </c>
       <c r="C57" s="5" t="s">
@@ -2542,7 +2569,7 @@
       </c>
     </row>
     <row r="58" spans="2:3">
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="18" t="s">
         <v>77</v>
       </c>
       <c r="C58" s="5" t="s">
@@ -2550,7 +2577,7 @@
       </c>
     </row>
     <row r="59" spans="2:5">
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="17" t="s">
         <v>79</v>
       </c>
       <c r="D59" s="8">
@@ -2564,7 +2591,7 @@
       <c r="A60" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="17" t="s">
         <v>74</v>
       </c>
       <c r="D60" s="8">
@@ -2575,10 +2602,10 @@
       </c>
     </row>
     <row r="61" spans="2:4">
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D61" s="15"/>
+      <c r="D61" s="17"/>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="5" t="s">
@@ -2603,7 +2630,7 @@
       </c>
     </row>
     <row r="64" spans="2:5">
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="17" t="s">
         <v>86</v>
       </c>
       <c r="D64" s="8">
@@ -2614,7 +2641,7 @@
       </c>
     </row>
     <row r="65" spans="2:5">
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="17" t="s">
         <v>87</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -2628,7 +2655,7 @@
       </c>
     </row>
     <row r="66" ht="28" spans="2:5">
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="16" t="s">
         <v>89</v>
       </c>
       <c r="D66" s="8">
@@ -2639,7 +2666,7 @@
       </c>
     </row>
     <row r="67" ht="28" spans="2:5">
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="18" t="s">
         <v>90</v>
       </c>
       <c r="D67" s="8">
@@ -2653,7 +2680,7 @@
       <c r="A68" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B68" s="15" t="s">
+      <c r="B68" s="17" t="s">
         <v>92</v>
       </c>
       <c r="D68" s="8">
@@ -2664,7 +2691,7 @@
       </c>
     </row>
     <row r="69" spans="2:5">
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="17" t="s">
         <v>93</v>
       </c>
       <c r="D69" s="8">
@@ -2722,7 +2749,7 @@
       </c>
     </row>
     <row r="74" spans="2:5">
-      <c r="B74" s="15" t="s">
+      <c r="B74" s="17" t="s">
         <v>99</v>
       </c>
       <c r="D74" s="8">
@@ -2777,16 +2804,16 @@
       </c>
     </row>
     <row r="79" spans="2:5">
-      <c r="B79" s="16" t="s">
+      <c r="B79" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="D79" s="20" t="s">
+      <c r="D79" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="E79" s="20"/>
+      <c r="E79" s="22"/>
     </row>
     <row r="80" spans="2:5">
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="18" t="s">
         <v>106</v>
       </c>
       <c r="D80" s="8">
@@ -2811,10 +2838,10 @@
       <c r="A82" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="B82" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="C82" s="15" t="s">
+      <c r="C82" s="17" t="s">
         <v>110</v>
       </c>
       <c r="D82" s="8">
@@ -2828,7 +2855,7 @@
       <c r="A83" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B83" s="17" t="s">
+      <c r="B83" s="19" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2841,7 +2868,7 @@
       <c r="A85" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B85" s="17"/>
+      <c r="B85" s="19"/>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="5" t="s">
@@ -2884,10 +2911,10 @@
       <c r="A91" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B91" s="15" t="s">
+      <c r="B91" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="C91" s="15" t="s">
+      <c r="C91" s="17" t="s">
         <v>124</v>
       </c>
       <c r="D91" s="8">
@@ -2915,7 +2942,7 @@
       <c r="A93" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B93" s="17" t="s">
         <v>128</v>
       </c>
       <c r="C93" s="5" t="s">
@@ -2929,7 +2956,7 @@
       </c>
     </row>
     <row r="95" spans="2:5">
-      <c r="B95" s="15" t="s">
+      <c r="B95" s="17" t="s">
         <v>130</v>
       </c>
       <c r="C95" s="5" t="s">
@@ -2946,13 +2973,13 @@
       <c r="A96" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B96" s="17" t="s">
+      <c r="B96" s="19" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="7"/>
-      <c r="B97" s="15" t="s">
+      <c r="B97" s="17" t="s">
         <v>134</v>
       </c>
       <c r="C97" s="5" t="s">
@@ -2979,7 +3006,7 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="7"/>
-      <c r="B99" s="15" t="s">
+      <c r="B99" s="17" t="s">
         <v>137</v>
       </c>
       <c r="D99" s="8">
@@ -2991,7 +3018,7 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="7"/>
-      <c r="B100" s="15" t="s">
+      <c r="B100" s="17" t="s">
         <v>138</v>
       </c>
       <c r="D100" s="8">
@@ -3003,7 +3030,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="7"/>
-      <c r="B101" s="15" t="s">
+      <c r="B101" s="17" t="s">
         <v>139</v>
       </c>
       <c r="D101" s="8">
@@ -3015,7 +3042,7 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="7"/>
-      <c r="B102" s="15" t="s">
+      <c r="B102" s="17" t="s">
         <v>140</v>
       </c>
       <c r="D102" s="8">
@@ -3027,10 +3054,10 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="7"/>
-      <c r="B103" s="17" t="s">
+      <c r="B103" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="C103" s="17" t="s">
+      <c r="C103" s="19" t="s">
         <v>142</v>
       </c>
       <c r="D103" s="8"/>
@@ -3038,7 +3065,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="7"/>
-      <c r="B104" s="15" t="s">
+      <c r="B104" s="17" t="s">
         <v>143</v>
       </c>
       <c r="C104" s="5" t="s">
@@ -3053,7 +3080,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="7"/>
-      <c r="B105" s="15" t="s">
+      <c r="B105" s="17" t="s">
         <v>145</v>
       </c>
       <c r="C105" s="5" t="s">
@@ -3068,16 +3095,16 @@
     </row>
     <row r="106" ht="28" spans="1:3">
       <c r="A106" s="7"/>
-      <c r="B106" s="16" t="s">
+      <c r="B106" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="C106" s="17" t="s">
+      <c r="C106" s="19" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="7"/>
-      <c r="B107" s="16" t="s">
+      <c r="B107" s="18" t="s">
         <v>149</v>
       </c>
       <c r="D107" s="8">
@@ -3089,13 +3116,13 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="7"/>
-      <c r="B108" s="21" t="s">
+      <c r="B108" s="18" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="7"/>
-      <c r="B109" s="15" t="s">
+      <c r="B109" s="17" t="s">
         <v>151</v>
       </c>
       <c r="D109" s="8">
@@ -3107,28 +3134,28 @@
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="7"/>
-      <c r="B110" s="15" t="s">
+      <c r="B110" s="17" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="7"/>
-      <c r="B111" s="15" t="s">
+      <c r="B111" s="17" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="7"/>
-      <c r="B112" s="15" t="s">
+      <c r="B112" s="17" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="7"/>
-      <c r="B113" s="15" t="s">
+      <c r="B113" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="C113" s="15" t="s">
+      <c r="C113" s="17" t="s">
         <v>156</v>
       </c>
       <c r="D113" s="8">
@@ -3140,7 +3167,7 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="7"/>
-      <c r="B114" s="15" t="s">
+      <c r="B114" s="17" t="s">
         <v>157</v>
       </c>
       <c r="C114" s="5" t="s">
@@ -3149,13 +3176,13 @@
     </row>
     <row r="115" ht="28" spans="1:2">
       <c r="A115" s="7"/>
-      <c r="B115" s="16" t="s">
+      <c r="B115" s="18" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="7"/>
-      <c r="B116" s="16" t="s">
+      <c r="B116" s="18" t="s">
         <v>159</v>
       </c>
       <c r="D116" s="8">
@@ -3167,7 +3194,7 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="7"/>
-      <c r="B117" s="15" t="s">
+      <c r="B117" s="17" t="s">
         <v>160</v>
       </c>
       <c r="D117" s="8">
@@ -3179,7 +3206,7 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="7"/>
-      <c r="B118" s="15" t="s">
+      <c r="B118" s="17" t="s">
         <v>161</v>
       </c>
       <c r="D118" s="8">
@@ -3191,7 +3218,7 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="7"/>
-      <c r="B119" s="22" t="s">
+      <c r="B119" s="17" t="s">
         <v>162</v>
       </c>
       <c r="C119" s="5" t="s">
@@ -3202,7 +3229,7 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="7"/>
-      <c r="B120" s="15" t="s">
+      <c r="B120" s="17" t="s">
         <v>164</v>
       </c>
       <c r="D120" s="8">
@@ -3214,7 +3241,7 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="7"/>
-      <c r="B121" s="15" t="s">
+      <c r="B121" s="17" t="s">
         <v>165</v>
       </c>
       <c r="D121" s="8">
@@ -3226,13 +3253,13 @@
     </row>
     <row r="122" spans="1:2">
       <c r="A122" s="7"/>
-      <c r="B122" s="17" t="s">
+      <c r="B122" s="19" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="123" ht="28" spans="1:5">
       <c r="A123" s="7"/>
-      <c r="B123" s="16" t="s">
+      <c r="B123" s="18" t="s">
         <v>167</v>
       </c>
       <c r="D123" s="8">
@@ -3270,10 +3297,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -3332,40 +3359,42 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" s="14" t="s">
         <v>174</v>
       </c>
+      <c r="B7" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="5" t="s">
-        <v>175</v>
-      </c>
+      <c r="A8" s="14"/>
       <c r="B8" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="5"/>
+      <c r="A9" s="14"/>
       <c r="B9" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="5"/>
+      <c r="A10" s="14"/>
       <c r="B10" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="5" t="s">
         <v>179</v>
       </c>
+      <c r="B11" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="5" t="s">
-        <v>180</v>
-      </c>
+      <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>181</v>
       </c>
@@ -3377,31 +3406,74 @@
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="5"/>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
+      <c r="A14" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" s="5" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="B15" t="s">
         <v>185</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="5"/>
+      <c r="B16" t="s">
         <v>186</v>
       </c>
     </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="5"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>189</v>
+      </c>
+      <c r="B20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="15"/>
+      <c r="B22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>194</v>
+      </c>
+      <c r="B23" t="s">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3430,16 +3502,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -3450,16 +3522,16 @@
     </row>
     <row r="2" ht="49" customHeight="1" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E2" s="8">
         <v>43867</v>
@@ -3470,16 +3542,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E3" s="8">
         <v>43877</v>
@@ -3490,32 +3562,32 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E5" s="8">
         <v>43877</v>
@@ -3526,16 +3598,16 @@
     </row>
     <row r="6" ht="37" customHeight="1" spans="1:6">
       <c r="A6" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>194</v>
       </c>
       <c r="E6" s="8">
         <v>43867</v>
@@ -3547,13 +3619,13 @@
     <row r="7" ht="48" customHeight="1" spans="1:6">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E7" s="8">
         <v>43867</v>
@@ -3564,16 +3636,16 @@
     </row>
     <row r="8" ht="43" customHeight="1" spans="1:6">
       <c r="A8" s="4" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E8" s="8">
         <v>43936</v>
@@ -3585,13 +3657,13 @@
     <row r="9" ht="37" customHeight="1" spans="1:6">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E9" s="8">
         <v>43936</v>
@@ -3602,16 +3674,16 @@
     </row>
     <row r="10" ht="59" customHeight="1" spans="1:6">
       <c r="A10" s="4" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="E10" s="8">
         <v>43876</v>
@@ -3653,16 +3725,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>3</v>
@@ -3673,16 +3745,16 @@
     </row>
     <row r="2" ht="42" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E2" s="8">
         <v>43867</v>
@@ -3693,16 +3765,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E3" s="8">
         <v>43877</v>
@@ -3713,32 +3785,32 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="C5" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E5" s="8">
         <v>43877</v>
@@ -3749,16 +3821,16 @@
     </row>
     <row r="6" ht="48" customHeight="1" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E6" s="8">
         <v>43867</v>
@@ -3769,13 +3841,13 @@
     </row>
     <row r="7" ht="45" customHeight="1" spans="2:6">
       <c r="B7" s="5" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E7" s="8">
         <v>43867</v>
@@ -3786,16 +3858,16 @@
     </row>
     <row r="8" ht="44" customHeight="1" spans="1:6">
       <c r="A8" s="5" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E8" s="8">
         <v>43936</v>
@@ -3806,13 +3878,13 @@
     </row>
     <row r="9" ht="47" customHeight="1" spans="2:6">
       <c r="B9" s="7" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E9" s="8">
         <v>43936</v>
@@ -3823,16 +3895,16 @@
     </row>
     <row r="10" ht="48" customHeight="1" spans="1:6">
       <c r="A10" s="5" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="E10" s="8">
         <v>43876</v>
@@ -3871,22 +3943,22 @@
   <sheetData>
     <row r="1" ht="23" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" ht="42" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" ht="121" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:1">

</xml_diff>

<commit_message>
[Author:z001 - Reason: 工作安排完善 - App]
</commit_message>
<xml_diff>
--- a/isoft_doc/工作安排.xlsx
+++ b/isoft_doc/工作安排.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7140"/>
+    <workbookView windowWidth="19200" windowHeight="7140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="web能力统计" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="237">
   <si>
     <t>模块</t>
   </si>
@@ -584,7 +584,10 @@
     <t>忘记密码和修改密码等功能</t>
   </si>
   <si>
-    <t>401 状态码全局拦截</t>
+    <t>401 状态码全局拦截：自动刷新 tokenString 弹框效果</t>
+  </si>
+  <si>
+    <t>401 状态码全局拦截：超过可刷新时间弹框前往登录</t>
   </si>
   <si>
     <t>课程详情页面</t>
@@ -636,6 +639,9 @@
   </si>
   <si>
     <t>分页方案优化</t>
+  </si>
+  <si>
+    <t>初次安装首页授权提示功能实现</t>
   </si>
   <si>
     <t>配置项</t>
@@ -880,10 +886,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -902,15 +908,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -918,6 +918,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -932,22 +947,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -962,7 +962,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -976,36 +983,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -1015,10 +992,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1031,10 +1008,39 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1078,67 +1084,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1150,43 +1126,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1210,19 +1150,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1234,7 +1180,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1246,19 +1252,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1272,17 +1278,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1305,8 +1311,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1316,41 +1322,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1369,6 +1340,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1377,149 +1383,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1561,6 +1567,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1933,8 +1942,8 @@
   <sheetPr/>
   <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2015,7 +2024,7 @@
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -2051,7 +2060,7 @@
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="8"/>
@@ -2083,7 +2092,7 @@
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="8">
@@ -2140,7 +2149,7 @@
       </c>
     </row>
     <row r="18" spans="2:2">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="16" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2204,7 +2213,7 @@
       </c>
     </row>
     <row r="26" ht="42" spans="2:5">
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="17" t="s">
         <v>35</v>
       </c>
       <c r="D26" s="8">
@@ -2215,10 +2224,10 @@
       </c>
     </row>
     <row r="27" ht="28" spans="2:5">
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="18" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="8">
@@ -2234,7 +2243,7 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="16" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="8">
@@ -2267,10 +2276,10 @@
       </c>
     </row>
     <row r="32" ht="56" spans="2:5">
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D32" s="8">
@@ -2314,7 +2323,7 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="16" t="s">
         <v>47</v>
       </c>
       <c r="D36" s="8">
@@ -2325,7 +2334,7 @@
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="17" t="s">
         <v>48</v>
       </c>
       <c r="D37" s="8">
@@ -2336,7 +2345,7 @@
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="17" t="s">
         <v>49</v>
       </c>
       <c r="D38" s="8">
@@ -2347,7 +2356,7 @@
       </c>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="17" t="s">
         <v>50</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -2397,7 +2406,7 @@
       </c>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="16" t="s">
         <v>56</v>
       </c>
       <c r="D43" s="8">
@@ -2408,10 +2417,10 @@
       </c>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="15"/>
+      <c r="C44" s="16"/>
       <c r="D44" s="8">
         <v>43896</v>
       </c>
@@ -2431,7 +2440,7 @@
       </c>
     </row>
     <row r="46" spans="2:5">
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C46" s="5" t="s">
@@ -2476,10 +2485,10 @@
       <c r="E49" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F49" s="15"/>
+      <c r="F49" s="16"/>
     </row>
     <row r="50" spans="2:6">
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="16" t="s">
         <v>64</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -2491,10 +2500,10 @@
       <c r="E50" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F50" s="15"/>
+      <c r="F50" s="16"/>
     </row>
     <row r="51" spans="2:6">
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="16" t="s">
         <v>66</v>
       </c>
       <c r="C51" s="5" t="s">
@@ -2506,7 +2515,7 @@
       <c r="E51" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F51" s="15"/>
+      <c r="F51" s="16"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="5" t="s">
@@ -2523,10 +2532,10 @@
       <c r="A53" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="20" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2539,7 +2548,7 @@
       <c r="A55" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="16" t="s">
         <v>73</v>
       </c>
       <c r="D55" s="8">
@@ -2550,15 +2559,15 @@
       </c>
     </row>
     <row r="56" spans="2:3">
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C56" s="20" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="57" ht="28" spans="2:3">
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="17" t="s">
         <v>75</v>
       </c>
       <c r="C57" s="5" t="s">
@@ -2566,7 +2575,7 @@
       </c>
     </row>
     <row r="58" spans="2:3">
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="17" t="s">
         <v>77</v>
       </c>
       <c r="C58" s="5" t="s">
@@ -2574,7 +2583,7 @@
       </c>
     </row>
     <row r="59" spans="2:5">
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="16" t="s">
         <v>79</v>
       </c>
       <c r="D59" s="8">
@@ -2588,7 +2597,7 @@
       <c r="A60" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="16" t="s">
         <v>74</v>
       </c>
       <c r="D60" s="8">
@@ -2599,10 +2608,10 @@
       </c>
     </row>
     <row r="61" spans="2:4">
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="D61" s="15"/>
+      <c r="D61" s="16"/>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="5" t="s">
@@ -2627,7 +2636,7 @@
       </c>
     </row>
     <row r="64" spans="2:5">
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="16" t="s">
         <v>86</v>
       </c>
       <c r="D64" s="8">
@@ -2638,7 +2647,7 @@
       </c>
     </row>
     <row r="65" spans="2:5">
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="16" t="s">
         <v>87</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -2652,7 +2661,7 @@
       </c>
     </row>
     <row r="66" ht="28" spans="2:5">
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="15" t="s">
         <v>89</v>
       </c>
       <c r="D66" s="8">
@@ -2663,7 +2672,7 @@
       </c>
     </row>
     <row r="67" ht="28" spans="2:5">
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="17" t="s">
         <v>90</v>
       </c>
       <c r="D67" s="8">
@@ -2677,7 +2686,7 @@
       <c r="A68" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B68" s="15" t="s">
+      <c r="B68" s="16" t="s">
         <v>92</v>
       </c>
       <c r="D68" s="8">
@@ -2688,7 +2697,7 @@
       </c>
     </row>
     <row r="69" spans="2:5">
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="16" t="s">
         <v>93</v>
       </c>
       <c r="D69" s="8">
@@ -2746,7 +2755,7 @@
       </c>
     </row>
     <row r="74" spans="2:5">
-      <c r="B74" s="15" t="s">
+      <c r="B74" s="16" t="s">
         <v>99</v>
       </c>
       <c r="D74" s="8">
@@ -2801,16 +2810,16 @@
       </c>
     </row>
     <row r="79" spans="2:5">
-      <c r="B79" s="16" t="s">
+      <c r="B79" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="D79" s="20" t="s">
+      <c r="D79" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="E79" s="20"/>
+      <c r="E79" s="21"/>
     </row>
     <row r="80" spans="2:5">
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="17" t="s">
         <v>106</v>
       </c>
       <c r="D80" s="8">
@@ -2835,10 +2844,10 @@
       <c r="A82" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="B82" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="C82" s="15" t="s">
+      <c r="C82" s="16" t="s">
         <v>110</v>
       </c>
       <c r="D82" s="8">
@@ -2852,7 +2861,7 @@
       <c r="A83" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B83" s="17" t="s">
+      <c r="B83" s="18" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2865,7 +2874,7 @@
       <c r="A85" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B85" s="17"/>
+      <c r="B85" s="18"/>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="5" t="s">
@@ -2908,10 +2917,10 @@
       <c r="A91" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B91" s="15" t="s">
+      <c r="B91" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C91" s="15" t="s">
+      <c r="C91" s="16" t="s">
         <v>124</v>
       </c>
       <c r="D91" s="8">
@@ -2939,7 +2948,7 @@
       <c r="A93" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B93" s="16" t="s">
         <v>128</v>
       </c>
       <c r="C93" s="5" t="s">
@@ -2953,7 +2962,7 @@
       </c>
     </row>
     <row r="95" spans="2:5">
-      <c r="B95" s="15" t="s">
+      <c r="B95" s="16" t="s">
         <v>130</v>
       </c>
       <c r="C95" s="5" t="s">
@@ -2970,13 +2979,13 @@
       <c r="A96" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B96" s="17" t="s">
+      <c r="B96" s="18" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="7"/>
-      <c r="B97" s="15" t="s">
+      <c r="B97" s="16" t="s">
         <v>134</v>
       </c>
       <c r="C97" s="5" t="s">
@@ -3003,7 +3012,7 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="7"/>
-      <c r="B99" s="15" t="s">
+      <c r="B99" s="16" t="s">
         <v>137</v>
       </c>
       <c r="D99" s="8">
@@ -3015,7 +3024,7 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="7"/>
-      <c r="B100" s="15" t="s">
+      <c r="B100" s="16" t="s">
         <v>138</v>
       </c>
       <c r="D100" s="8">
@@ -3027,7 +3036,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="7"/>
-      <c r="B101" s="15" t="s">
+      <c r="B101" s="16" t="s">
         <v>139</v>
       </c>
       <c r="D101" s="8">
@@ -3039,7 +3048,7 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="7"/>
-      <c r="B102" s="15" t="s">
+      <c r="B102" s="16" t="s">
         <v>140</v>
       </c>
       <c r="D102" s="8">
@@ -3051,10 +3060,10 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="7"/>
-      <c r="B103" s="17" t="s">
+      <c r="B103" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="C103" s="17" t="s">
+      <c r="C103" s="18" t="s">
         <v>142</v>
       </c>
       <c r="D103" s="8"/>
@@ -3062,7 +3071,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="7"/>
-      <c r="B104" s="15" t="s">
+      <c r="B104" s="16" t="s">
         <v>143</v>
       </c>
       <c r="C104" s="5" t="s">
@@ -3077,7 +3086,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="7"/>
-      <c r="B105" s="15" t="s">
+      <c r="B105" s="16" t="s">
         <v>145</v>
       </c>
       <c r="C105" s="5" t="s">
@@ -3092,16 +3101,16 @@
     </row>
     <row r="106" ht="28" spans="1:3">
       <c r="A106" s="7"/>
-      <c r="B106" s="16" t="s">
+      <c r="B106" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="C106" s="17" t="s">
+      <c r="C106" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="7"/>
-      <c r="B107" s="16" t="s">
+      <c r="B107" s="17" t="s">
         <v>149</v>
       </c>
       <c r="D107" s="8">
@@ -3113,13 +3122,13 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="7"/>
-      <c r="B108" s="16" t="s">
+      <c r="B108" s="17" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="7"/>
-      <c r="B109" s="15" t="s">
+      <c r="B109" s="16" t="s">
         <v>151</v>
       </c>
       <c r="D109" s="8">
@@ -3131,28 +3140,28 @@
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="7"/>
-      <c r="B110" s="15" t="s">
+      <c r="B110" s="16" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="7"/>
-      <c r="B111" s="15" t="s">
+      <c r="B111" s="16" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="7"/>
-      <c r="B112" s="15" t="s">
+      <c r="B112" s="16" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="7"/>
-      <c r="B113" s="15" t="s">
+      <c r="B113" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="C113" s="15" t="s">
+      <c r="C113" s="16" t="s">
         <v>156</v>
       </c>
       <c r="D113" s="8">
@@ -3164,7 +3173,7 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="7"/>
-      <c r="B114" s="15" t="s">
+      <c r="B114" s="16" t="s">
         <v>157</v>
       </c>
       <c r="C114" s="5" t="s">
@@ -3173,13 +3182,13 @@
     </row>
     <row r="115" ht="28" spans="1:2">
       <c r="A115" s="7"/>
-      <c r="B115" s="16" t="s">
+      <c r="B115" s="17" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="7"/>
-      <c r="B116" s="16" t="s">
+      <c r="B116" s="17" t="s">
         <v>159</v>
       </c>
       <c r="D116" s="8">
@@ -3191,7 +3200,7 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="7"/>
-      <c r="B117" s="15" t="s">
+      <c r="B117" s="16" t="s">
         <v>160</v>
       </c>
       <c r="D117" s="8">
@@ -3203,7 +3212,7 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="7"/>
-      <c r="B118" s="15" t="s">
+      <c r="B118" s="16" t="s">
         <v>161</v>
       </c>
       <c r="D118" s="8">
@@ -3215,7 +3224,7 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="7"/>
-      <c r="B119" s="15" t="s">
+      <c r="B119" s="16" t="s">
         <v>162</v>
       </c>
       <c r="C119" s="5" t="s">
@@ -3226,7 +3235,7 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="7"/>
-      <c r="B120" s="15" t="s">
+      <c r="B120" s="16" t="s">
         <v>164</v>
       </c>
       <c r="D120" s="8">
@@ -3238,7 +3247,7 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="7"/>
-      <c r="B121" s="15" t="s">
+      <c r="B121" s="16" t="s">
         <v>165</v>
       </c>
       <c r="D121" s="8">
@@ -3250,7 +3259,7 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="7"/>
-      <c r="B122" s="15" t="s">
+      <c r="B122" s="16" t="s">
         <v>166</v>
       </c>
       <c r="C122" s="5" t="s">
@@ -3265,7 +3274,7 @@
     </row>
     <row r="123" ht="28" spans="1:5">
       <c r="A123" s="7"/>
-      <c r="B123" s="16" t="s">
+      <c r="B123" s="17" t="s">
         <v>168</v>
       </c>
       <c r="D123" s="8">
@@ -3303,16 +3312,16 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="29.4545454545455" customWidth="1"/>
-    <col min="2" max="2" width="40.3636363636364" customWidth="1"/>
+    <col min="2" max="2" width="55.1818181818182" customWidth="1"/>
     <col min="3" max="3" width="23.3636363636364" customWidth="1"/>
     <col min="4" max="4" width="31.1818181818182" customWidth="1"/>
     <col min="5" max="5" width="20.0909090909091" customWidth="1"/>
@@ -3392,15 +3401,15 @@
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s">
         <v>180</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="5" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="5"/>
       <c r="B12" t="s">
         <v>182</v>
       </c>
@@ -3411,75 +3420,88 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" s="5"/>
+      <c r="B14" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="5" t="s">
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
         <v>185</v>
       </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="5" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="5"/>
       <c r="B16" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:2">
       <c r="A17" s="5"/>
+      <c r="B17" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>188</v>
-      </c>
+      <c r="A18" s="5"/>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>190</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="5" t="s">
+      <c r="B21" t="s">
         <v>192</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="5" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="5"/>
       <c r="B22" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" t="s">
+      <c r="A23" s="5"/>
+      <c r="B23" t="s">
         <v>195</v>
       </c>
-      <c r="B23" t="s">
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="14" t="s">
         <v>196</v>
       </c>
+      <c r="B24" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="14"/>
+      <c r="B25" t="s">
+        <v>198</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3508,16 +3530,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -3528,16 +3550,16 @@
     </row>
     <row r="2" ht="49" customHeight="1" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E2" s="8">
         <v>43867</v>
@@ -3548,16 +3570,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="E3" s="8">
         <v>43877</v>
@@ -3568,32 +3590,32 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E5" s="8">
         <v>43877</v>
@@ -3604,16 +3626,16 @@
     </row>
     <row r="6" ht="37" customHeight="1" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E6" s="8">
         <v>43867</v>
@@ -3625,13 +3647,13 @@
     <row r="7" ht="48" customHeight="1" spans="1:6">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E7" s="8">
         <v>43867</v>
@@ -3642,16 +3664,16 @@
     </row>
     <row r="8" ht="43" customHeight="1" spans="1:6">
       <c r="A8" s="4" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E8" s="8">
         <v>43936</v>
@@ -3663,13 +3685,13 @@
     <row r="9" ht="37" customHeight="1" spans="1:6">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E9" s="8">
         <v>43936</v>
@@ -3680,16 +3702,16 @@
     </row>
     <row r="10" ht="59" customHeight="1" spans="1:6">
       <c r="A10" s="4" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E10" s="8">
         <v>43876</v>
@@ -3731,16 +3753,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>3</v>
@@ -3751,16 +3773,16 @@
     </row>
     <row r="2" ht="42" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E2" s="8">
         <v>43867</v>
@@ -3771,16 +3793,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E3" s="8">
         <v>43877</v>
@@ -3791,32 +3813,32 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C5" t="s">
         <v>212</v>
       </c>
-      <c r="C5" t="s">
-        <v>210</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E5" s="8">
         <v>43877</v>
@@ -3827,16 +3849,16 @@
     </row>
     <row r="6" ht="48" customHeight="1" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E6" s="8">
         <v>43867</v>
@@ -3847,13 +3869,13 @@
     </row>
     <row r="7" ht="45" customHeight="1" spans="2:6">
       <c r="B7" s="5" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E7" s="8">
         <v>43867</v>
@@ -3864,16 +3886,16 @@
     </row>
     <row r="8" ht="44" customHeight="1" spans="1:6">
       <c r="A8" s="5" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>229</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>227</v>
       </c>
       <c r="E8" s="8">
         <v>43936</v>
@@ -3884,13 +3906,13 @@
     </row>
     <row r="9" ht="47" customHeight="1" spans="2:6">
       <c r="B9" s="7" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E9" s="8">
         <v>43936</v>
@@ -3901,16 +3923,16 @@
     </row>
     <row r="10" ht="48" customHeight="1" spans="1:6">
       <c r="A10" s="5" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E10" s="8">
         <v>43876</v>
@@ -3949,22 +3971,22 @@
   <sheetData>
     <row r="1" ht="23" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" ht="42" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" ht="121" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:1">

</xml_diff>

<commit_message>
[Author:z001 - Reason: 需求分析、进度补充]
</commit_message>
<xml_diff>
--- a/isoft_doc/工作安排.xlsx
+++ b/isoft_doc/工作安排.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="254">
   <si>
     <t>模块</t>
   </si>
@@ -557,9 +557,18 @@
     <t>开屏广告页</t>
   </si>
   <si>
+    <t>添加广告功能</t>
+  </si>
+  <si>
+    <t>商业合作跳转</t>
+  </si>
+  <si>
     <t>首页</t>
   </si>
   <si>
+    <t>权限申请（目前文件存储权限）</t>
+  </si>
+  <si>
     <t>首页侧边栏分类</t>
   </si>
   <si>
@@ -590,12 +599,27 @@
     <t>401 状态码全局拦截：超过可刷新时间弹框前往登录</t>
   </si>
   <si>
+    <t>下单确认页面</t>
+  </si>
+  <si>
+    <t>支付页面</t>
+  </si>
+  <si>
+    <t>订单列表页面</t>
+  </si>
+  <si>
+    <t>订单详情页面</t>
+  </si>
+  <si>
     <t>课程详情页面</t>
   </si>
   <si>
     <t>课程详情展示</t>
   </si>
   <si>
+    <t>样式优化</t>
+  </si>
+  <si>
     <t>课程收藏、点赞功能展示</t>
   </si>
   <si>
@@ -617,7 +641,7 @@
     <t>课程推荐页面</t>
   </si>
   <si>
-    <t>课程搜索页面</t>
+    <t>.</t>
   </si>
   <si>
     <t>功能列表页面</t>
@@ -642,6 +666,33 @@
   </si>
   <si>
     <t>初次安装首页授权提示功能实现</t>
+  </si>
+  <si>
+    <t>推荐页面</t>
+  </si>
+  <si>
+    <t>轮播图（优惠券入口、学习线路图入口）</t>
+  </si>
+  <si>
+    <t>购物车</t>
+  </si>
+  <si>
+    <t>暂时不做</t>
+  </si>
+  <si>
+    <t>我的片段页面</t>
+  </si>
+  <si>
+    <t>中间图标菜单（5个，目前设置优惠券和订单、消息）</t>
+  </si>
+  <si>
+    <t>检查更新：上线前实现</t>
+  </si>
+  <si>
+    <t>设置页面</t>
+  </si>
+  <si>
+    <t>关于页面</t>
   </si>
   <si>
     <t>配置项</t>
@@ -886,12 +937,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -905,6 +956,13 @@
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -924,7 +982,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -934,6 +1014,14 @@
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -961,53 +1049,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1030,17 +1074,31 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1051,12 +1109,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1084,61 +1148,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1150,31 +1160,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1192,7 +1178,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1204,13 +1196,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1222,49 +1298,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1279,6 +1343,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1289,6 +1377,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1336,45 +1439,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1383,10 +1447,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1395,137 +1459,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1568,6 +1632,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1577,16 +1653,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1940,7 +2016,7 @@
   <dimension ref="A1:F123"/>
   <sheetViews>
     <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+      <selection activeCell="D104" sqref="D104:D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -2021,7 +2097,7 @@
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="18" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -2057,7 +2133,7 @@
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="19" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="8"/>
@@ -2089,7 +2165,7 @@
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="8">
@@ -2146,7 +2222,7 @@
       </c>
     </row>
     <row r="18" spans="2:2">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="19" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2210,7 +2286,7 @@
       </c>
     </row>
     <row r="26" ht="42" spans="2:5">
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="20" t="s">
         <v>35</v>
       </c>
       <c r="D26" s="8">
@@ -2221,10 +2297,10 @@
       </c>
     </row>
     <row r="27" ht="28" spans="2:5">
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="21" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="8">
@@ -2240,7 +2316,7 @@
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="19" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="8">
@@ -2273,10 +2349,10 @@
       </c>
     </row>
     <row r="32" ht="56" spans="2:5">
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="21" t="s">
         <v>43</v>
       </c>
       <c r="D32" s="8">
@@ -2320,7 +2396,7 @@
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="19" t="s">
         <v>47</v>
       </c>
       <c r="D36" s="8">
@@ -2331,7 +2407,7 @@
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="20" t="s">
         <v>48</v>
       </c>
       <c r="D37" s="8">
@@ -2342,7 +2418,7 @@
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="20" t="s">
         <v>49</v>
       </c>
       <c r="D38" s="8">
@@ -2353,7 +2429,7 @@
       </c>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="20" t="s">
         <v>50</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -2403,7 +2479,7 @@
       </c>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="19" t="s">
         <v>56</v>
       </c>
       <c r="D43" s="8">
@@ -2414,10 +2490,10 @@
       </c>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="15"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="8">
         <v>43896</v>
       </c>
@@ -2437,7 +2513,7 @@
       </c>
     </row>
     <row r="46" spans="2:5">
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="19" t="s">
         <v>59</v>
       </c>
       <c r="C46" s="5" t="s">
@@ -2482,10 +2558,10 @@
       <c r="E49" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F49" s="15"/>
+      <c r="F49" s="19"/>
     </row>
     <row r="50" spans="2:6">
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="19" t="s">
         <v>64</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -2497,10 +2573,10 @@
       <c r="E50" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F50" s="15"/>
+      <c r="F50" s="19"/>
     </row>
     <row r="51" spans="2:6">
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="19" t="s">
         <v>66</v>
       </c>
       <c r="C51" s="5" t="s">
@@ -2512,7 +2588,7 @@
       <c r="E51" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F51" s="15"/>
+      <c r="F51" s="19"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="5" t="s">
@@ -2529,10 +2605,10 @@
       <c r="A53" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="23" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2545,7 +2621,7 @@
       <c r="A55" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="19" t="s">
         <v>73</v>
       </c>
       <c r="D55" s="8">
@@ -2556,15 +2632,15 @@
       </c>
     </row>
     <row r="56" spans="2:3">
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C56" s="23" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="57" ht="28" spans="2:3">
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="20" t="s">
         <v>75</v>
       </c>
       <c r="C57" s="5" t="s">
@@ -2572,7 +2648,7 @@
       </c>
     </row>
     <row r="58" spans="2:3">
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="20" t="s">
         <v>77</v>
       </c>
       <c r="C58" s="5" t="s">
@@ -2580,7 +2656,7 @@
       </c>
     </row>
     <row r="59" spans="2:5">
-      <c r="B59" s="15" t="s">
+      <c r="B59" s="19" t="s">
         <v>79</v>
       </c>
       <c r="D59" s="8">
@@ -2594,7 +2670,7 @@
       <c r="A60" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="19" t="s">
         <v>74</v>
       </c>
       <c r="D60" s="8">
@@ -2605,10 +2681,10 @@
       </c>
     </row>
     <row r="61" spans="2:4">
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="D61" s="15"/>
+      <c r="D61" s="19"/>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="5" t="s">
@@ -2633,7 +2709,7 @@
       </c>
     </row>
     <row r="64" spans="2:5">
-      <c r="B64" s="15" t="s">
+      <c r="B64" s="19" t="s">
         <v>86</v>
       </c>
       <c r="D64" s="8">
@@ -2644,7 +2720,7 @@
       </c>
     </row>
     <row r="65" spans="2:5">
-      <c r="B65" s="15" t="s">
+      <c r="B65" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C65" s="5" t="s">
@@ -2658,7 +2734,7 @@
       </c>
     </row>
     <row r="66" ht="28" spans="2:5">
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="18" t="s">
         <v>89</v>
       </c>
       <c r="D66" s="8">
@@ -2669,7 +2745,7 @@
       </c>
     </row>
     <row r="67" ht="28" spans="2:5">
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="20" t="s">
         <v>90</v>
       </c>
       <c r="D67" s="8">
@@ -2683,7 +2759,7 @@
       <c r="A68" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B68" s="15" t="s">
+      <c r="B68" s="19" t="s">
         <v>92</v>
       </c>
       <c r="D68" s="8">
@@ -2694,7 +2770,7 @@
       </c>
     </row>
     <row r="69" spans="2:5">
-      <c r="B69" s="15" t="s">
+      <c r="B69" s="19" t="s">
         <v>93</v>
       </c>
       <c r="D69" s="8">
@@ -2752,7 +2828,7 @@
       </c>
     </row>
     <row r="74" spans="2:5">
-      <c r="B74" s="15" t="s">
+      <c r="B74" s="19" t="s">
         <v>99</v>
       </c>
       <c r="D74" s="8">
@@ -2807,16 +2883,16 @@
       </c>
     </row>
     <row r="79" spans="2:5">
-      <c r="B79" s="16" t="s">
+      <c r="B79" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D79" s="20" t="s">
+      <c r="D79" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="E79" s="20"/>
+      <c r="E79" s="24"/>
     </row>
     <row r="80" spans="2:5">
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="20" t="s">
         <v>106</v>
       </c>
       <c r="D80" s="8">
@@ -2841,10 +2917,10 @@
       <c r="A82" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="B82" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C82" s="15" t="s">
+      <c r="C82" s="19" t="s">
         <v>110</v>
       </c>
       <c r="D82" s="8">
@@ -2858,7 +2934,7 @@
       <c r="A83" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B83" s="17" t="s">
+      <c r="B83" s="21" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2871,7 +2947,7 @@
       <c r="A85" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B85" s="17"/>
+      <c r="B85" s="21"/>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="5" t="s">
@@ -2914,10 +2990,10 @@
       <c r="A91" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B91" s="15" t="s">
+      <c r="B91" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="C91" s="15" t="s">
+      <c r="C91" s="19" t="s">
         <v>124</v>
       </c>
       <c r="D91" s="8">
@@ -2945,7 +3021,7 @@
       <c r="A93" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B93" s="15" t="s">
+      <c r="B93" s="19" t="s">
         <v>128</v>
       </c>
       <c r="C93" s="5" t="s">
@@ -2959,7 +3035,7 @@
       </c>
     </row>
     <row r="95" spans="2:5">
-      <c r="B95" s="15" t="s">
+      <c r="B95" s="19" t="s">
         <v>130</v>
       </c>
       <c r="C95" s="5" t="s">
@@ -2976,13 +3052,13 @@
       <c r="A96" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B96" s="17" t="s">
+      <c r="B96" s="21" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="7"/>
-      <c r="B97" s="15" t="s">
+      <c r="B97" s="19" t="s">
         <v>134</v>
       </c>
       <c r="C97" s="5" t="s">
@@ -3009,7 +3085,7 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="7"/>
-      <c r="B99" s="15" t="s">
+      <c r="B99" s="19" t="s">
         <v>137</v>
       </c>
       <c r="D99" s="8">
@@ -3021,7 +3097,7 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="7"/>
-      <c r="B100" s="15" t="s">
+      <c r="B100" s="19" t="s">
         <v>138</v>
       </c>
       <c r="D100" s="8">
@@ -3033,7 +3109,7 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="7"/>
-      <c r="B101" s="15" t="s">
+      <c r="B101" s="19" t="s">
         <v>139</v>
       </c>
       <c r="D101" s="8">
@@ -3045,7 +3121,7 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="7"/>
-      <c r="B102" s="15" t="s">
+      <c r="B102" s="19" t="s">
         <v>140</v>
       </c>
       <c r="D102" s="8">
@@ -3057,10 +3133,10 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="7"/>
-      <c r="B103" s="17" t="s">
+      <c r="B103" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="C103" s="17" t="s">
+      <c r="C103" s="21" t="s">
         <v>142</v>
       </c>
       <c r="D103" s="8"/>
@@ -3068,7 +3144,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="7"/>
-      <c r="B104" s="15" t="s">
+      <c r="B104" s="19" t="s">
         <v>143</v>
       </c>
       <c r="C104" s="5" t="s">
@@ -3083,7 +3159,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="7"/>
-      <c r="B105" s="15" t="s">
+      <c r="B105" s="19" t="s">
         <v>145</v>
       </c>
       <c r="C105" s="5" t="s">
@@ -3098,16 +3174,16 @@
     </row>
     <row r="106" ht="28" spans="1:3">
       <c r="A106" s="7"/>
-      <c r="B106" s="16" t="s">
+      <c r="B106" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="C106" s="17" t="s">
+      <c r="C106" s="21" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="7"/>
-      <c r="B107" s="16" t="s">
+      <c r="B107" s="20" t="s">
         <v>149</v>
       </c>
       <c r="D107" s="8">
@@ -3119,13 +3195,13 @@
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="7"/>
-      <c r="B108" s="16" t="s">
+      <c r="B108" s="20" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="7"/>
-      <c r="B109" s="15" t="s">
+      <c r="B109" s="19" t="s">
         <v>151</v>
       </c>
       <c r="D109" s="8">
@@ -3137,28 +3213,28 @@
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="7"/>
-      <c r="B110" s="15" t="s">
+      <c r="B110" s="19" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="7"/>
-      <c r="B111" s="15" t="s">
+      <c r="B111" s="19" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" s="7"/>
-      <c r="B112" s="15" t="s">
+      <c r="B112" s="19" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="7"/>
-      <c r="B113" s="15" t="s">
+      <c r="B113" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="C113" s="15" t="s">
+      <c r="C113" s="19" t="s">
         <v>156</v>
       </c>
       <c r="D113" s="8">
@@ -3170,7 +3246,7 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="7"/>
-      <c r="B114" s="15" t="s">
+      <c r="B114" s="19" t="s">
         <v>157</v>
       </c>
       <c r="C114" s="5" t="s">
@@ -3179,13 +3255,13 @@
     </row>
     <row r="115" ht="28" spans="1:2">
       <c r="A115" s="7"/>
-      <c r="B115" s="16" t="s">
+      <c r="B115" s="20" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="7"/>
-      <c r="B116" s="16" t="s">
+      <c r="B116" s="20" t="s">
         <v>159</v>
       </c>
       <c r="D116" s="8">
@@ -3197,7 +3273,7 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="7"/>
-      <c r="B117" s="15" t="s">
+      <c r="B117" s="19" t="s">
         <v>160</v>
       </c>
       <c r="D117" s="8">
@@ -3209,7 +3285,7 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="7"/>
-      <c r="B118" s="15" t="s">
+      <c r="B118" s="19" t="s">
         <v>161</v>
       </c>
       <c r="D118" s="8">
@@ -3221,7 +3297,7 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="7"/>
-      <c r="B119" s="15" t="s">
+      <c r="B119" s="19" t="s">
         <v>162</v>
       </c>
       <c r="C119" s="5" t="s">
@@ -3232,7 +3308,7 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="7"/>
-      <c r="B120" s="15" t="s">
+      <c r="B120" s="19" t="s">
         <v>164</v>
       </c>
       <c r="D120" s="8">
@@ -3244,7 +3320,7 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="7"/>
-      <c r="B121" s="15" t="s">
+      <c r="B121" s="19" t="s">
         <v>165</v>
       </c>
       <c r="D121" s="8">
@@ -3256,7 +3332,7 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="7"/>
-      <c r="B122" s="15" t="s">
+      <c r="B122" s="19" t="s">
         <v>166</v>
       </c>
       <c r="C122" s="5" t="s">
@@ -3271,7 +3347,7 @@
     </row>
     <row r="123" ht="28" spans="1:5">
       <c r="A123" s="7"/>
-      <c r="B123" s="16" t="s">
+      <c r="B123" s="20" t="s">
         <v>168</v>
       </c>
       <c r="D123" s="8">
@@ -3309,10 +3385,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -3341,164 +3417,294 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" s="14" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="B2" s="5" t="s">
         <v>170</v>
       </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="15"/>
+      <c r="B3" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="5" t="s">
-        <v>171</v>
+      <c r="A4" t="s">
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="5"/>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="5" t="s">
+        <v>174</v>
+      </c>
       <c r="B5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>175</v>
+      </c>
+      <c r="D5" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E5" s="16"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="5"/>
       <c r="B6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
-        <v>175</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="D6" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E6" s="16"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="5"/>
+        <v>177</v>
+      </c>
+      <c r="D7" s="8">
+        <v>43986</v>
+      </c>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="5" t="s">
+        <v>178</v>
+      </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>179</v>
+      </c>
+      <c r="D8" s="8">
+        <v>43986</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="5"/>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="5"/>
       <c r="B10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="5"/>
       <c r="B11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="5" t="s">
-        <v>181</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="D11" s="17">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="5"/>
       <c r="B12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="5"/>
-      <c r="B13" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="5"/>
-      <c r="B14" t="s">
+      <c r="D12" s="17">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="5" t="s">
         <v>184</v>
       </c>
     </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
     <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="A15" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
       <c r="A16" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="B16" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="5"/>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="B17" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>189</v>
+      </c>
+      <c r="C17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="5"/>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B18" t="s">
+        <v>191</v>
+      </c>
+      <c r="C18" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5"/>
+      <c r="B19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>193</v>
+      </c>
+      <c r="C20" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>191</v>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5" t="s">
+        <v>194</v>
       </c>
       <c r="B21" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="5" t="s">
-        <v>193</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="C21" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5"/>
       <c r="B22" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>196</v>
+      </c>
+      <c r="C22" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
       <c r="A23" s="5"/>
-      <c r="B23" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="5"/>
-      <c r="B25" t="s">
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
         <v>198</v>
       </c>
     </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>199</v>
+      </c>
+      <c r="B26" t="s">
+        <v>200</v>
+      </c>
+      <c r="D26" s="17">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B27" t="s">
+        <v>202</v>
+      </c>
+      <c r="D27" s="17">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="5"/>
+      <c r="B28" t="s">
+        <v>203</v>
+      </c>
+      <c r="D28" s="17">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D29" s="17">
+        <v>43986</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="5"/>
+      <c r="B30" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B31" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>209</v>
+      </c>
+      <c r="B32" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="B33" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="14"/>
+      <c r="B34" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="14"/>
+      <c r="B35" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="14"/>
+      <c r="B36" t="s">
+        <v>215</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
+  <mergeCells count="8">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A33:A36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3527,16 +3733,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -3547,16 +3753,16 @@
     </row>
     <row r="2" ht="49" customHeight="1" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="E2" s="8">
         <v>43867</v>
@@ -3567,16 +3773,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="E3" s="8">
         <v>43877</v>
@@ -3587,32 +3793,32 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="E5" s="8">
         <v>43877</v>
@@ -3623,16 +3829,16 @@
     </row>
     <row r="6" ht="37" customHeight="1" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="E6" s="8">
         <v>43867</v>
@@ -3644,13 +3850,13 @@
     <row r="7" ht="48" customHeight="1" spans="1:6">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>218</v>
+        <v>235</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>219</v>
+        <v>236</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="E7" s="8">
         <v>43867</v>
@@ -3661,16 +3867,16 @@
     </row>
     <row r="8" ht="43" customHeight="1" spans="1:6">
       <c r="A8" s="4" t="s">
-        <v>220</v>
+        <v>237</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="E8" s="8">
         <v>43936</v>
@@ -3682,13 +3888,13 @@
     <row r="9" ht="37" customHeight="1" spans="1:6">
       <c r="A9" s="4"/>
       <c r="B9" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>206</v>
       </c>
       <c r="E9" s="8">
         <v>43936</v>
@@ -3699,16 +3905,16 @@
     </row>
     <row r="10" ht="59" customHeight="1" spans="1:6">
       <c r="A10" s="4" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="E10" s="8">
         <v>43876</v>
@@ -3750,16 +3956,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>3</v>
@@ -3770,16 +3976,16 @@
     </row>
     <row r="2" ht="42" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="E2" s="8">
         <v>43867</v>
@@ -3790,16 +3996,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>230</v>
+        <v>247</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="E3" s="8">
         <v>43877</v>
@@ -3810,32 +4016,32 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="5" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="B5" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="C5" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="E5" s="8">
         <v>43877</v>
@@ -3846,16 +4052,16 @@
     </row>
     <row r="6" ht="48" customHeight="1" spans="1:6">
       <c r="A6" s="5" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="E6" s="8">
         <v>43867</v>
@@ -3866,13 +4072,13 @@
     </row>
     <row r="7" ht="45" customHeight="1" spans="2:6">
       <c r="B7" s="5" t="s">
-        <v>218</v>
+        <v>235</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>219</v>
+        <v>236</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="E7" s="8">
         <v>43867</v>
@@ -3883,16 +4089,16 @@
     </row>
     <row r="8" ht="44" customHeight="1" spans="1:6">
       <c r="A8" s="5" t="s">
-        <v>220</v>
+        <v>237</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>231</v>
+        <v>248</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="E8" s="8">
         <v>43936</v>
@@ -3903,13 +4109,13 @@
     </row>
     <row r="9" ht="47" customHeight="1" spans="2:6">
       <c r="B9" s="7" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="E9" s="8">
         <v>43936</v>
@@ -3920,16 +4126,16 @@
     </row>
     <row r="10" ht="48" customHeight="1" spans="1:6">
       <c r="A10" s="5" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="E10" s="8">
         <v>43876</v>
@@ -3968,22 +4174,22 @@
   <sheetData>
     <row r="1" ht="23" customHeight="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" ht="42" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" ht="121" customHeight="1" spans="1:1">
       <c r="A4" s="3" t="s">
-        <v>236</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:1">

</xml_diff>

<commit_message>
[Author:z001 - Reason: 资料完善]
</commit_message>
<xml_diff>
--- a/isoft_doc/工作安排.xlsx
+++ b/isoft_doc/工作安排.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7130" firstSheet="1" activeTab="7"/>
+    <workbookView windowWidth="23040" windowHeight="9420" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="web能力统计" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="未来规划" sheetId="6" r:id="rId6"/>
     <sheet name="微信开发平台" sheetId="8" r:id="rId7"/>
     <sheet name="录屏软件" sheetId="9" r:id="rId8"/>
+    <sheet name="git账号" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">web能力统计!$A$1:$F$131</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="332">
   <si>
     <t>模块</t>
   </si>
@@ -1182,6 +1183,24 @@
   <si>
     <t>嗨格式录屏录屏登录账号：18255005137，密码：linkknown2020    支持5台电脑同时在线录制</t>
   </si>
+  <si>
+    <t>账号</t>
+  </si>
+  <si>
+    <t>密码</t>
+  </si>
+  <si>
+    <t>邮箱</t>
+  </si>
+  <si>
+    <t>linkknown</t>
+  </si>
+  <si>
+    <t>linkknown2020</t>
+  </si>
+  <si>
+    <t>linkknown@163.com</t>
+  </si>
 </sst>
 </file>
 
@@ -1189,9 +1208,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1231,8 +1250,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1254,9 +1312,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1264,28 +1321,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1306,9 +1341,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1322,31 +1357,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1398,13 +1417,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1416,133 +1537,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1560,25 +1555,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1592,26 +1611,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1651,11 +1661,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1675,17 +1691,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1697,10 +1716,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1709,16 +1728,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1727,120 +1746,123 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -2295,1401 +2317,1401 @@
       <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="17.4545454545455" style="5" customWidth="1"/>
-    <col min="2" max="2" width="72.3636363636364" style="5" customWidth="1"/>
-    <col min="3" max="3" width="34.2727272727273" style="5" customWidth="1"/>
-    <col min="4" max="4" width="22.6363636363636" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.0909090909091" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="5"/>
+    <col min="1" max="1" width="17.4537037037037" style="6" customWidth="1"/>
+    <col min="2" max="2" width="72.3611111111111" style="6" customWidth="1"/>
+    <col min="3" max="3" width="34.2685185185185" style="6" customWidth="1"/>
+    <col min="4" max="4" width="22.6388888888889" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10.0925925925926" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="9">
         <v>43867</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" ht="28" spans="2:5">
-      <c r="B3" s="7" t="s">
+      <c r="E2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" ht="28.8" spans="2:5">
+      <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="9">
         <v>43870</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="9">
         <v>43871</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="9">
         <v>44004</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" ht="28" spans="2:5">
-      <c r="B6" s="7" t="s">
+      <c r="E5" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" ht="28.8" spans="2:5">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="9">
         <v>43890</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" ht="56" spans="1:5">
-      <c r="A7" s="5" t="s">
+      <c r="E6" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" ht="57.6" spans="1:5">
+      <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="9">
         <v>43911</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="9">
         <v>43885</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="9">
         <v>43885</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="9">
         <v>43885</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="9">
         <v>43870</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="9">
         <v>43911</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="9">
         <v>43911</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="9">
         <v>43885</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" ht="56" spans="1:5">
-      <c r="A16" s="5" t="s">
+      <c r="E15" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" ht="57.6" spans="1:5">
+      <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="9">
         <v>43875</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:2">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="2:2">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:2">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="23" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="8">
+      <c r="C20" s="28"/>
+      <c r="D20" s="9">
         <v>44006</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="9">
         <v>43879</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="9">
         <v>43879</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="9">
         <v>43890</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="2:2">
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="9">
         <v>43908</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" ht="42" spans="2:5">
-      <c r="B28" s="28" t="s">
+      <c r="E27" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" ht="43.2" spans="2:5">
+      <c r="B28" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="9">
         <v>43914</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" ht="28" spans="2:2">
-      <c r="B29" s="28" t="s">
+      <c r="E28" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" ht="28.8" spans="2:2">
+      <c r="B29" s="29" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="8">
+      <c r="D30" s="9">
         <v>43888</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="9">
         <v>43879</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="9">
         <v>43879</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="8">
+      <c r="D33" s="9">
         <v>43919</v>
       </c>
-      <c r="E33" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" ht="56" spans="2:5">
-      <c r="B34" s="28" t="s">
+      <c r="E33" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" ht="57.6" spans="2:5">
+      <c r="B34" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="9">
         <v>43888</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" ht="28" spans="2:5">
-      <c r="B35" s="7" t="s">
+      <c r="E34" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" ht="28.8" spans="2:5">
+      <c r="B35" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="9">
         <v>43888</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="9">
         <v>43888</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="9">
         <v>43888</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D38" s="9">
         <v>43898</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E38" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D39" s="9">
         <v>43946</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="2:5">
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D40" s="8">
+      <c r="D40" s="9">
         <v>43951</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D41" s="9">
         <v>43888</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D42" s="9">
         <v>43879</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E42" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="8">
+      <c r="D43" s="9">
         <v>43896</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D44" s="9">
         <v>43896</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="45" spans="2:5">
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="22"/>
-      <c r="D45" s="8">
+      <c r="C45" s="23"/>
+      <c r="D45" s="9">
         <v>43896</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="46" spans="2:5">
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D46" s="9">
         <v>43896</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="47" spans="2:5">
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D47" s="9">
         <v>43896</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="2:5">
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="D48" s="8">
+      <c r="D48" s="9">
         <v>43891</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E48" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="2:5">
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D49" s="8">
+      <c r="D49" s="9">
         <v>43889</v>
       </c>
-      <c r="E49" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" ht="28" spans="2:6">
-      <c r="B50" s="7" t="s">
+      <c r="E49" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" ht="28.8" spans="2:6">
+      <c r="B50" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="8">
+      <c r="D50" s="9">
         <v>43889</v>
       </c>
-      <c r="E50" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" s="22"/>
+      <c r="E50" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="23"/>
     </row>
     <row r="51" spans="2:6">
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D51" s="8">
+      <c r="D51" s="9">
         <v>43947</v>
       </c>
-      <c r="E51" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F51" s="22"/>
+      <c r="E51" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="23"/>
     </row>
     <row r="52" spans="2:6">
-      <c r="B52" s="22" t="s">
+      <c r="B52" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D52" s="8">
+      <c r="D52" s="9">
         <v>43947</v>
       </c>
-      <c r="E52" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F52" s="22"/>
+      <c r="E52" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="23"/>
     </row>
     <row r="53" spans="2:5">
-      <c r="B53" s="22" t="s">
+      <c r="B53" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D53" s="8">
+      <c r="D53" s="9">
         <v>43888</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E53" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C54" s="30" t="s">
+      <c r="C54" s="31" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="55" spans="2:2">
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="23" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D56" s="8">
+      <c r="D56" s="9">
         <v>43898</v>
       </c>
-      <c r="E56" s="9" t="s">
+      <c r="E56" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="57" spans="2:3">
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C57" s="30" t="s">
+      <c r="C57" s="31" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="58" spans="2:3">
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="59" ht="28" spans="2:3">
-      <c r="B59" s="28" t="s">
+    <row r="59" ht="28.8" spans="2:3">
+      <c r="B59" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="60" spans="2:5">
-      <c r="B60" s="28" t="s">
+      <c r="B60" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="D60" s="8">
+      <c r="D60" s="9">
         <v>43897</v>
       </c>
-      <c r="E60" s="9" t="s">
+      <c r="E60" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B61" s="22" t="s">
+      <c r="B61" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D61" s="8">
+      <c r="D61" s="9">
         <v>43908</v>
       </c>
-      <c r="E61" s="9" t="s">
+      <c r="E61" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="62" spans="2:4">
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="D62" s="22"/>
+      <c r="D62" s="23"/>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="23" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D64" s="8">
+      <c r="D64" s="9">
         <v>43879</v>
       </c>
-      <c r="E64" s="9" t="s">
+      <c r="E64" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="65" spans="2:5">
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D65" s="8">
+      <c r="D65" s="9">
         <v>43879</v>
       </c>
-      <c r="E65" s="9" t="s">
+      <c r="E65" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="66" spans="2:5">
-      <c r="B66" s="22" t="s">
+      <c r="B66" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D66" s="8">
+      <c r="D66" s="9">
         <v>43953</v>
       </c>
-      <c r="E66" s="9" t="s">
+      <c r="E66" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="67" spans="2:5">
-      <c r="B67" s="22" t="s">
+      <c r="B67" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D67" s="8">
+      <c r="D67" s="9">
         <v>43940</v>
       </c>
-      <c r="E67" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="68" ht="28" spans="2:2">
-      <c r="B68" s="26" t="s">
+      <c r="E67" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" ht="28.8" spans="2:2">
+      <c r="B68" s="27" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="69" spans="2:5">
-      <c r="B69" s="31" t="s">
+      <c r="B69" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D69" s="8">
+      <c r="D69" s="9">
         <v>43893</v>
       </c>
-      <c r="E69" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" ht="28" spans="1:5">
-      <c r="A70" s="5" t="s">
+      <c r="E69" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" ht="28.8" spans="1:5">
+      <c r="A70" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B70" s="28" t="s">
+      <c r="B70" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="D70" s="8">
+      <c r="D70" s="9">
         <v>43939</v>
       </c>
-      <c r="E70" s="9" t="s">
+      <c r="E70" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="71" spans="2:5">
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="D71" s="8">
+      <c r="D71" s="9">
         <v>43940</v>
       </c>
-      <c r="E71" s="9" t="s">
+      <c r="E71" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B72" s="22" t="s">
+      <c r="B72" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="D72" s="8">
+      <c r="D72" s="9">
         <v>43873</v>
       </c>
-      <c r="E72" s="9" t="s">
+      <c r="E72" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="73" spans="2:5">
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D73" s="8">
+      <c r="D73" s="9">
         <v>43873</v>
       </c>
-      <c r="E73" s="9" t="s">
+      <c r="E73" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="74" spans="2:5">
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="D74" s="8">
+      <c r="D74" s="9">
         <v>43873</v>
       </c>
-      <c r="E74" s="9" t="s">
+      <c r="E74" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="75" spans="2:5">
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D75" s="8">
+      <c r="D75" s="9">
         <v>43873</v>
       </c>
-      <c r="E75" s="9" t="s">
+      <c r="E75" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="76" spans="2:5">
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D76" s="8">
+      <c r="D76" s="9">
         <v>43940</v>
       </c>
-      <c r="E76" s="9" t="s">
+      <c r="E76" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="77" spans="2:5">
-      <c r="B77" s="22" t="s">
+      <c r="B77" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="D77" s="8">
+      <c r="D77" s="9">
         <v>43873</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="E77" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="78" spans="2:5">
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D78" s="8">
+      <c r="D78" s="9">
         <v>43873</v>
       </c>
-      <c r="E78" s="9" t="s">
+      <c r="E78" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="79" spans="2:5">
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D79" s="8">
+      <c r="D79" s="9">
         <v>43873</v>
       </c>
-      <c r="E79" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="80" ht="28" spans="2:5">
-      <c r="B80" s="7" t="s">
+      <c r="E79" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" ht="28.8" spans="2:5">
+      <c r="B80" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D80" s="8">
+      <c r="D80" s="9">
         <v>43873</v>
       </c>
-      <c r="E80" s="9" t="s">
+      <c r="E80" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="81" spans="2:5">
-      <c r="B81" s="7" t="s">
+      <c r="B81" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D81" s="32" t="s">
+      <c r="D81" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="E81" s="32"/>
+      <c r="E81" s="33"/>
     </row>
     <row r="82" spans="2:5">
-      <c r="B82" s="28" t="s">
+      <c r="B82" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="D82" s="8">
+      <c r="D82" s="9">
         <v>43904</v>
       </c>
-      <c r="E82" s="9" t="s">
+      <c r="E82" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="83" spans="2:5">
-      <c r="B83" s="28" t="s">
+      <c r="B83" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="D83" s="8">
+      <c r="D83" s="9">
         <v>43873</v>
       </c>
-      <c r="E83" s="9" t="s">
+      <c r="E83" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C84" s="22" t="s">
+      <c r="C84" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="D84" s="8">
+      <c r="D84" s="9">
         <v>43953</v>
       </c>
-      <c r="E84" s="9" t="s">
+      <c r="E84" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:2">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="B85" s="22" t="s">
+      <c r="B85" s="23" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:2">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B86" s="24" t="s">
+      <c r="B86" s="25" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="6" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D88" s="8">
+      <c r="D88" s="9">
         <v>43868</v>
       </c>
-      <c r="E88" s="9" t="s">
+      <c r="E88" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:2">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="6" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="90" spans="2:2">
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="6" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="6" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="6" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="6" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="6" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="95" spans="1:5">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B95" s="22" t="s">
+      <c r="B95" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D95" s="8">
+      <c r="D95" s="9">
         <v>44005</v>
       </c>
-      <c r="E95" s="9" t="s">
+      <c r="E95" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="5" t="s">
+      <c r="A96" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C96" s="22" t="s">
+      <c r="C96" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="D96" s="8">
+      <c r="D96" s="9">
         <v>43967</v>
       </c>
-      <c r="E96" s="9" t="s">
+      <c r="E96" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B97" s="22" t="s">
+      <c r="B97" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="D97" s="8">
+      <c r="D97" s="9">
         <v>43881</v>
       </c>
-      <c r="E97" s="9" t="s">
+      <c r="E97" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="5" t="s">
+      <c r="A98" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C98" s="5" t="s">
+      <c r="C98" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D98" s="8">
+      <c r="D98" s="9">
         <v>43966</v>
       </c>
-      <c r="E98" s="9" t="s">
+      <c r="E98" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="99" spans="2:2">
-      <c r="B99" s="22" t="s">
+      <c r="B99" s="23" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="100" spans="3:5">
-      <c r="C100" s="5" t="s">
+      <c r="C100" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="D100" s="8">
+      <c r="D100" s="9">
         <v>43952</v>
       </c>
-      <c r="E100" s="9" t="s">
+      <c r="E100" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:2">
-      <c r="A101" s="7" t="s">
+      <c r="A101" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B101" s="22" t="s">
+      <c r="B101" s="23" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="102" spans="1:5">
-      <c r="A102" s="7"/>
-      <c r="B102" s="24" t="s">
+      <c r="A102" s="8"/>
+      <c r="B102" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="C102" s="5" t="s">
+      <c r="C102" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D102" s="8">
+      <c r="D102" s="9">
         <v>43953</v>
       </c>
-      <c r="E102" s="9" t="s">
+      <c r="E102" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="7"/>
-      <c r="B103" s="22" t="s">
+      <c r="A103" s="8"/>
+      <c r="B103" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="D103" s="8">
+      <c r="D103" s="9">
         <v>43894</v>
       </c>
-      <c r="E103" s="9" t="s">
+      <c r="E103" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="7"/>
-      <c r="B104" s="5" t="s">
+      <c r="A104" s="8"/>
+      <c r="B104" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D104" s="8">
+      <c r="D104" s="9">
         <v>43888</v>
       </c>
-      <c r="E104" s="9" t="s">
+      <c r="E104" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="7"/>
-      <c r="B105" s="22" t="s">
+      <c r="A105" s="8"/>
+      <c r="B105" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="D105" s="8">
+      <c r="D105" s="9">
         <v>43919</v>
       </c>
-      <c r="E105" s="9" t="s">
+      <c r="E105" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="7"/>
-      <c r="B106" s="22" t="s">
+      <c r="A106" s="8"/>
+      <c r="B106" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="D106" s="8">
+      <c r="D106" s="9">
         <v>43890</v>
       </c>
-      <c r="E106" s="9" t="s">
+      <c r="E106" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="7"/>
-      <c r="B107" s="22" t="s">
+      <c r="A107" s="8"/>
+      <c r="B107" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="D107" s="8">
+      <c r="D107" s="9">
         <v>43881</v>
       </c>
-      <c r="E107" s="9" t="s">
+      <c r="E107" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="7"/>
-      <c r="B108" s="22" t="s">
+      <c r="A108" s="8"/>
+      <c r="B108" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="C108" s="24" t="s">
+      <c r="C108" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="D108" s="8"/>
-      <c r="E108" s="9"/>
+      <c r="D108" s="9"/>
+      <c r="E108" s="10"/>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="7"/>
-      <c r="B109" s="24" t="s">
+      <c r="A109" s="8"/>
+      <c r="B109" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C109" s="5" t="s">
+      <c r="C109" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="D109" s="8">
+      <c r="D109" s="9">
         <v>43940</v>
       </c>
-      <c r="E109" s="9" t="s">
+      <c r="E109" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="110" spans="1:5">
-      <c r="A110" s="7"/>
-      <c r="B110" s="22" t="s">
+      <c r="A110" s="8"/>
+      <c r="B110" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="C110" s="5" t="s">
+      <c r="C110" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="D110" s="8">
+      <c r="D110" s="9">
         <v>43904</v>
       </c>
-      <c r="E110" s="9" t="s">
+      <c r="E110" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="111" spans="1:3">
-      <c r="A111" s="7"/>
-      <c r="B111" s="22" t="s">
+      <c r="A111" s="8"/>
+      <c r="B111" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="C111" s="24" t="s">
+      <c r="C111" s="25" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="112" ht="28" spans="1:5">
-      <c r="A112" s="7"/>
-      <c r="B112" s="28" t="s">
+    <row r="112" ht="28.8" spans="1:5">
+      <c r="A112" s="8"/>
+      <c r="B112" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="D112" s="8">
+      <c r="D112" s="9">
         <v>43919</v>
       </c>
-      <c r="E112" s="9" t="s">
+      <c r="E112" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="113" spans="1:2">
-      <c r="A113" s="7"/>
-      <c r="B113" s="28" t="s">
+      <c r="A113" s="8"/>
+      <c r="B113" s="29" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="114" spans="1:5">
-      <c r="A114" s="7"/>
-      <c r="B114" s="28" t="s">
+      <c r="A114" s="8"/>
+      <c r="B114" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="D114" s="8">
+      <c r="D114" s="9">
         <v>43904</v>
       </c>
-      <c r="E114" s="9" t="s">
+      <c r="E114" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="115" spans="1:2">
-      <c r="A115" s="7"/>
-      <c r="B115" s="22" t="s">
+      <c r="A115" s="8"/>
+      <c r="B115" s="23" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="116" spans="1:2">
-      <c r="A116" s="7"/>
-      <c r="B116" s="22" t="s">
+      <c r="A116" s="8"/>
+      <c r="B116" s="23" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="117" spans="1:2">
-      <c r="A117" s="7"/>
-      <c r="B117" s="22" t="s">
+      <c r="A117" s="8"/>
+      <c r="B117" s="23" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="118" spans="1:5">
-      <c r="A118" s="7"/>
-      <c r="B118" s="22" t="s">
+      <c r="A118" s="8"/>
+      <c r="B118" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="C118" s="22" t="s">
+      <c r="C118" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="D118" s="8">
+      <c r="D118" s="9">
         <v>43963</v>
       </c>
-      <c r="E118" s="9" t="s">
+      <c r="E118" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="119" spans="1:3">
-      <c r="A119" s="7"/>
-      <c r="B119" s="22" t="s">
+      <c r="A119" s="8"/>
+      <c r="B119" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="C119" s="5" t="s">
+      <c r="C119" s="6" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="120" spans="1:2">
-      <c r="A120" s="7"/>
-      <c r="B120" s="22" t="s">
+      <c r="A120" s="8"/>
+      <c r="B120" s="23" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="121" spans="1:2">
-      <c r="A121" s="7"/>
-      <c r="B121" s="20" t="s">
+      <c r="A121" s="8"/>
+      <c r="B121" s="21" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="122" ht="28" spans="1:5">
-      <c r="A122" s="7"/>
-      <c r="B122" s="28" t="s">
+    <row r="122" ht="28.8" spans="1:5">
+      <c r="A122" s="8"/>
+      <c r="B122" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="D122" s="8">
+      <c r="D122" s="9">
         <v>43953</v>
       </c>
-      <c r="E122" s="9" t="s">
+      <c r="E122" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="123" spans="1:5">
-      <c r="A123" s="7"/>
-      <c r="B123" s="28" t="s">
+      <c r="A123" s="8"/>
+      <c r="B123" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="D123" s="8">
+      <c r="D123" s="9">
         <v>43953</v>
       </c>
-      <c r="E123" s="9" t="s">
+      <c r="E123" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="124" spans="1:5">
-      <c r="A124" s="7"/>
-      <c r="B124" s="22" t="s">
+      <c r="A124" s="8"/>
+      <c r="B124" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="D124" s="8">
+      <c r="D124" s="9">
         <v>43953</v>
       </c>
-      <c r="E124" s="9" t="s">
+      <c r="E124" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" s="7"/>
-      <c r="B125" s="22" t="s">
+      <c r="A125" s="8"/>
+      <c r="B125" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="C125" s="5" t="s">
+      <c r="C125" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D125" s="8"/>
-      <c r="E125" s="9"/>
+      <c r="D125" s="9"/>
+      <c r="E125" s="10"/>
     </row>
     <row r="126" spans="1:5">
-      <c r="A126" s="7"/>
-      <c r="B126" s="22" t="s">
+      <c r="A126" s="8"/>
+      <c r="B126" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="D126" s="8">
+      <c r="D126" s="9">
         <v>43940</v>
       </c>
-      <c r="E126" s="9" t="s">
+      <c r="E126" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="127" spans="1:5">
-      <c r="A127" s="7"/>
-      <c r="B127" s="22" t="s">
+      <c r="A127" s="8"/>
+      <c r="B127" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="D127" s="8">
+      <c r="D127" s="9">
         <v>43963</v>
       </c>
-      <c r="E127" s="9" t="s">
+      <c r="E127" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="128" spans="1:5">
-      <c r="A128" s="7"/>
-      <c r="B128" s="22" t="s">
+      <c r="A128" s="8"/>
+      <c r="B128" s="23" t="s">
         <v>173</v>
       </c>
-      <c r="C128" s="5" t="s">
+      <c r="C128" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D128" s="8">
+      <c r="D128" s="9">
         <v>43968</v>
       </c>
-      <c r="E128" s="9" t="s">
+      <c r="E128" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="129" spans="1:4">
-      <c r="A129" s="7"/>
-      <c r="B129" s="22" t="s">
+      <c r="A129" s="8"/>
+      <c r="B129" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="D129" s="22"/>
+      <c r="D129" s="23"/>
     </row>
     <row r="130" spans="1:5">
-      <c r="A130" s="7"/>
-      <c r="B130" s="24" t="s">
+      <c r="A130" s="8"/>
+      <c r="B130" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="D130" s="8">
+      <c r="D130" s="9">
         <v>43953</v>
       </c>
-      <c r="E130" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="131" ht="28" spans="2:2">
-      <c r="B131" s="28" t="s">
+      <c r="E130" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" ht="28.8" spans="2:2">
+      <c r="B131" s="29" t="s">
         <v>177</v>
       </c>
     </row>
@@ -3724,1009 +3746,1009 @@
   <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.73148148148148" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.8181818181818" customWidth="1"/>
-    <col min="2" max="2" width="16.6363636363636" customWidth="1"/>
-    <col min="3" max="3" width="11.4545454545455" customWidth="1"/>
-    <col min="4" max="4" width="51.4545454545455" customWidth="1"/>
-    <col min="5" max="5" width="16.1818181818182" customWidth="1"/>
-    <col min="6" max="6" width="17.1818181818182" customWidth="1"/>
-    <col min="7" max="7" width="31.7272727272727" customWidth="1"/>
-    <col min="8" max="8" width="15.9090909090909" customWidth="1"/>
-    <col min="9" max="9" width="13.5454545454545" customWidth="1"/>
+    <col min="1" max="1" width="15.8148148148148" customWidth="1"/>
+    <col min="2" max="2" width="16.6388888888889" customWidth="1"/>
+    <col min="3" max="3" width="11.4537037037037" customWidth="1"/>
+    <col min="4" max="4" width="51.4537037037037" customWidth="1"/>
+    <col min="5" max="5" width="16.1851851851852" customWidth="1"/>
+    <col min="6" max="6" width="17.1851851851852" customWidth="1"/>
+    <col min="7" max="7" width="31.7314814814815" customWidth="1"/>
+    <col min="8" max="8" width="15.9074074074074" customWidth="1"/>
+    <col min="9" max="9" width="13.5462962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="5"/>
+      <c r="A3" s="6"/>
       <c r="D3" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>186</v>
       </c>
       <c r="D4" t="s">
         <v>187</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="9">
         <v>43986</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="5"/>
-      <c r="D5" s="15" t="s">
+      <c r="A5" s="6"/>
+      <c r="D5" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="H5" s="8">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="H5" s="9">
         <v>43992</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="5"/>
+      <c r="A6" s="6"/>
       <c r="D6" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="5"/>
+      <c r="A7" s="6"/>
       <c r="D7" t="s">
         <v>190</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="9">
         <v>43986</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="5"/>
+      <c r="A8" s="6"/>
       <c r="D8" t="s">
         <v>191</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="9">
         <v>43986</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>192</v>
       </c>
       <c r="B9" t="s">
         <v>193</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="H9" s="8">
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="H9" s="9">
         <v>43991</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="5"/>
+      <c r="A10" s="6"/>
       <c r="B10" t="s">
         <v>195</v>
       </c>
       <c r="D10" t="s">
         <v>195</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="9">
         <v>43991</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="5"/>
+      <c r="A11" s="6"/>
       <c r="B11" t="s">
         <v>127</v>
       </c>
       <c r="D11" t="s">
         <v>127</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="9">
         <v>43991</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="5"/>
+      <c r="A12" s="6"/>
       <c r="B12" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="8">
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="9">
         <v>43990</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="5"/>
+      <c r="A13" s="6"/>
       <c r="B13" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="8">
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="9">
         <v>43994</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="5"/>
+      <c r="A14" s="6"/>
       <c r="B14" t="s">
         <v>198</v>
       </c>
       <c r="D14" t="s">
         <v>199</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="8">
+      <c r="G14" s="16"/>
+      <c r="H14" s="9">
         <v>43990</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="5"/>
+      <c r="A15" s="6"/>
       <c r="B15" t="s">
         <v>200</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="H15" s="15"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="6" t="s">
         <v>204</v>
       </c>
       <c r="D16" t="s">
         <v>205</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="9">
         <v>43990</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
       <c r="D17" t="s">
         <v>206</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="9">
         <v>43990</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="15" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
       <c r="G18" t="s">
         <v>208</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="9">
         <v>43997</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="15" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="H19" s="8">
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="H19" s="9">
         <v>44006</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="15" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="H20" s="8">
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="H20" s="9">
         <v>43987</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="15" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="H21" s="8">
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="H21" s="9">
         <v>43987</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I21" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
       <c r="C22" t="s">
         <v>211</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
       <c r="G22" t="s">
         <v>213</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="9">
         <v>43998</v>
       </c>
-      <c r="I22" s="9" t="s">
+      <c r="I22" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="18" t="s">
         <v>215</v>
       </c>
       <c r="D23" t="s">
         <v>216</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="9">
         <v>43993</v>
       </c>
-      <c r="I23" s="9" t="s">
+      <c r="I23" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="16" t="s">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="H24" s="18"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
       <c r="C25" t="s">
         <v>218</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="H25" s="8">
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="H25" s="9">
         <v>43991</v>
       </c>
-      <c r="I25" s="9" t="s">
+      <c r="I25" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
       <c r="C26" t="s">
         <v>220</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="H26" s="18"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="H26" s="19"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="5"/>
-      <c r="B27" s="20" t="s">
+      <c r="A27" s="6"/>
+      <c r="B27" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="H27" s="18"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="H27" s="19"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="5"/>
-      <c r="B28" s="20"/>
-      <c r="H28" s="18"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="21"/>
+      <c r="H28" s="19"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="5"/>
+      <c r="A29" s="6"/>
       <c r="B29" t="s">
         <v>224</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="8">
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="9">
         <v>43992</v>
       </c>
-      <c r="I29" s="9" t="s">
+      <c r="I29" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="6" t="s">
         <v>226</v>
       </c>
       <c r="B30" t="s">
         <v>227</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="H30" s="8">
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="H30" s="9">
         <v>43994</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="I30" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="5"/>
+      <c r="A31" s="6"/>
       <c r="B31" t="s">
         <v>229</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="16" t="s">
         <v>230</v>
       </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="H31" s="8">
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="H31" s="9">
         <v>43994</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="I31" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="6" t="s">
         <v>126</v>
       </c>
       <c r="B32" t="s">
         <v>231</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="H32" s="8">
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="H32" s="9">
         <v>43991</v>
       </c>
-      <c r="I32" s="9" t="s">
+      <c r="I32" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="5"/>
+      <c r="A33" s="6"/>
       <c r="B33" t="s">
         <v>233</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="5"/>
+      <c r="A34" s="6"/>
       <c r="B34" t="s">
         <v>235</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="H34" s="8">
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="H34" s="9">
         <v>44004</v>
       </c>
-      <c r="I34" s="9" t="s">
+      <c r="I34" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5" t="s">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="16" t="s">
         <v>238</v>
       </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="H35" s="8">
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="H35" s="9">
         <v>44004</v>
       </c>
-      <c r="I35" s="9" t="s">
+      <c r="I35" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="D36" s="15" t="s">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="D36" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
       <c r="G36" t="s">
         <v>240</v>
       </c>
-      <c r="H36" s="8">
+      <c r="H36" s="9">
         <v>43992</v>
       </c>
-      <c r="I36" s="9" t="s">
+      <c r="I36" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="5"/>
+      <c r="A37" s="6"/>
       <c r="B37" t="s">
         <v>241</v>
       </c>
       <c r="G37" t="s">
         <v>240</v>
       </c>
-      <c r="H37" s="8">
+      <c r="H37" s="9">
         <v>43993</v>
       </c>
-      <c r="I37" s="9" t="s">
+      <c r="I37" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="5"/>
+      <c r="A38" s="6"/>
       <c r="B38" t="s">
         <v>242</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H38" s="9">
         <v>43993</v>
       </c>
-      <c r="I38" s="9" t="s">
+      <c r="I38" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="5"/>
+      <c r="A39" s="6"/>
       <c r="B39" t="s">
         <v>243</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="H39" s="18"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="H39" s="19"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="5"/>
+      <c r="A40" s="6"/>
       <c r="B40" t="s">
         <v>245</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="H40" s="18"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="H40" s="19"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="5"/>
+      <c r="A41" s="6"/>
       <c r="B41" t="s">
         <v>127</v>
       </c>
       <c r="G41" t="s">
         <v>240</v>
       </c>
-      <c r="H41" s="8">
+      <c r="H41" s="9">
         <v>43993</v>
       </c>
-      <c r="I41" s="9" t="s">
+      <c r="I41" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5" t="s">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6" t="s">
         <v>247</v>
       </c>
       <c r="C42" t="s">
         <v>248</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="H42" s="8">
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="H42" s="9">
         <v>43991</v>
       </c>
-      <c r="I42" s="9" t="s">
+      <c r="I42" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
       <c r="C43" t="s">
         <v>249</v>
       </c>
-      <c r="D43" s="22" t="s">
+      <c r="D43" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="H43" s="8">
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="H43" s="9">
         <v>43991</v>
       </c>
-      <c r="I43" s="9" t="s">
+      <c r="I43" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
       <c r="C44" t="s">
         <v>250</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="D44" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="H44" s="8">
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="H44" s="9">
         <v>43991</v>
       </c>
-      <c r="I44" s="9" t="s">
+      <c r="I44" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
       <c r="C45" t="s">
         <v>251</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-      <c r="H45" s="8">
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="H45" s="9">
         <v>43991</v>
       </c>
-      <c r="I45" s="9" t="s">
+      <c r="I45" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="5"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
       <c r="C46" t="s">
         <v>252</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="H46" s="8">
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="H46" s="9">
         <v>43991</v>
       </c>
-      <c r="I46" s="9" t="s">
+      <c r="I46" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5" t="s">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="H47" s="8">
+      <c r="E47" s="23"/>
+      <c r="F47" s="23"/>
+      <c r="H47" s="9">
         <v>43991</v>
       </c>
-      <c r="I47" s="9" t="s">
+      <c r="I47" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5" t="s">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6" t="s">
         <v>255</v>
       </c>
       <c r="C48" t="s">
         <v>256</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="H48" s="8">
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="H48" s="9">
         <v>44001</v>
       </c>
-      <c r="I48" s="9" t="s">
+      <c r="I48" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
       <c r="C49" t="s">
         <v>258</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="E49" s="15"/>
-      <c r="F49" s="15"/>
-      <c r="H49" s="8">
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="H49" s="9">
         <v>43993</v>
       </c>
-      <c r="I49" s="9" t="s">
+      <c r="I49" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
       <c r="C50" t="s">
         <v>260</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="H50" s="8">
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="H50" s="9">
         <v>43993</v>
       </c>
-      <c r="I50" s="9" t="s">
+      <c r="I50" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
       <c r="C51" t="s">
         <v>262</v>
       </c>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="H51" s="8">
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="H51" s="9">
         <v>43991</v>
       </c>
-      <c r="I51" s="9" t="s">
+      <c r="I51" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
       <c r="C52" t="s">
         <v>263</v>
       </c>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="H52" s="8">
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="H52" s="9">
         <v>43991</v>
       </c>
-      <c r="I52" s="9" t="s">
+      <c r="I52" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
       <c r="C53" t="s">
         <v>264</v>
       </c>
-      <c r="H53" s="8">
+      <c r="H53" s="9">
         <v>43991</v>
       </c>
-      <c r="I53" s="9" t="s">
+      <c r="I53" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="5"/>
+      <c r="A54" s="6"/>
       <c r="B54" t="s">
         <v>265</v>
       </c>
-      <c r="H54" s="8">
+      <c r="H54" s="9">
         <v>43991</v>
       </c>
-      <c r="I54" s="9" t="s">
+      <c r="I54" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="5"/>
+      <c r="A55" s="6"/>
       <c r="B55" t="s">
         <v>266</v>
       </c>
       <c r="D55" t="s">
         <v>267</v>
       </c>
-      <c r="H55" s="8">
+      <c r="H55" s="9">
         <v>43991</v>
       </c>
-      <c r="I55" s="9" t="s">
+      <c r="I55" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="16" t="s">
         <v>268</v>
       </c>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-      <c r="H56" s="8">
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="H56" s="9">
         <v>44005</v>
       </c>
-      <c r="I56" s="9" t="s">
+      <c r="I56" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="5"/>
-      <c r="D57" s="16" t="s">
+      <c r="A57" s="6"/>
+      <c r="D57" s="17" t="s">
         <v>269</v>
       </c>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="H57" s="18"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="H57" s="19"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="5"/>
-      <c r="D58" s="16" t="s">
+      <c r="A58" s="6"/>
+      <c r="D58" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="H58" s="18"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17"/>
+      <c r="H58" s="19"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="H59" s="18"/>
+      <c r="A59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="H59" s="19"/>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="5"/>
+      <c r="A60" s="6"/>
       <c r="B60" t="s">
         <v>271</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="D60" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="E60" s="22"/>
-      <c r="F60" s="22"/>
-      <c r="G60" s="15" t="s">
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="16" t="s">
         <v>273</v>
       </c>
-      <c r="H60" s="8">
+      <c r="H60" s="9">
         <v>43997</v>
       </c>
-      <c r="I60" s="9" t="s">
+      <c r="I60" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="5"/>
+      <c r="A61" s="6"/>
       <c r="B61" t="s">
         <v>274</v>
       </c>
-      <c r="D61" s="23" t="s">
+      <c r="D61" s="24" t="s">
         <v>275</v>
       </c>
-      <c r="E61" s="23"/>
-      <c r="F61" s="23"/>
-      <c r="H61" s="18"/>
+      <c r="E61" s="24"/>
+      <c r="F61" s="24"/>
+      <c r="H61" s="19"/>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="5"/>
+      <c r="A62" s="6"/>
       <c r="B62" t="s">
         <v>276</v>
       </c>
-      <c r="H62" s="18"/>
+      <c r="H62" s="19"/>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="5"/>
-      <c r="B63" s="16" t="s">
+      <c r="A63" s="6"/>
+      <c r="B63" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="H63" s="18"/>
+      <c r="H63" s="19"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="5"/>
+      <c r="A64" s="6"/>
       <c r="B64" t="s">
         <v>278</v>
       </c>
-      <c r="D64" s="24" t="s">
+      <c r="D64" s="25" t="s">
         <v>279</v>
       </c>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24"/>
-      <c r="H64" s="18"/>
+      <c r="E64" s="25"/>
+      <c r="F64" s="25"/>
+      <c r="H64" s="19"/>
     </row>
     <row r="65" spans="1:8">
-      <c r="A65" s="5"/>
-      <c r="D65" s="25" t="s">
+      <c r="A65" s="6"/>
+      <c r="D65" s="26" t="s">
         <v>280</v>
       </c>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="H65" s="18"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="H65" s="19"/>
     </row>
     <row r="66" spans="4:6">
-      <c r="D66" s="15" t="s">
+      <c r="D66" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
     </row>
     <row r="67" spans="4:6">
-      <c r="D67" s="15" t="s">
+      <c r="D67" s="16" t="s">
         <v>282</v>
       </c>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
     </row>
     <row r="68" spans="4:6">
-      <c r="D68" s="16" t="s">
+      <c r="D68" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I68">
@@ -4763,206 +4785,206 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.73148148148148" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="20" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.0909090909091" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.6363636363636" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.4545454545455" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.2727272727273" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.72727272727273" style="1"/>
+    <col min="1" max="1" width="20" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.0925925925926" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.6388888888889" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.4537037037037" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.2685185185185" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.73148148148148" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" ht="49" customHeight="1" spans="1:6">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>289</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="9">
         <v>43867</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="9">
         <v>43877</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="12"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="9">
         <v>43877</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" ht="37" customHeight="1" spans="1:6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="9">
         <v>43867</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" ht="48" customHeight="1" spans="1:6">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>304</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="9">
         <v>43867</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" ht="43" customHeight="1" spans="1:6">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>307</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="9">
         <v>43936</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" ht="37" customHeight="1" spans="1:6">
-      <c r="A9" s="4"/>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="9">
         <v>43936</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" ht="59" customHeight="1" spans="1:6">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="9">
         <v>43876</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4984,97 +5006,97 @@
   <sheetPr/>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.73148148148148" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="20.3636363636364" style="5" customWidth="1"/>
+    <col min="1" max="1" width="20.3611111111111" style="6" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="3" max="3" width="48.5454545454545" customWidth="1"/>
-    <col min="4" max="4" width="13.1818181818182" customWidth="1"/>
+    <col min="3" max="3" width="48.5462962962963" customWidth="1"/>
+    <col min="4" max="4" width="13.1851851851852" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="42" spans="1:6">
-      <c r="A2" s="5" t="s">
+    <row r="2" ht="43.2" spans="1:6">
+      <c r="A2" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="9">
         <v>43867</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="9">
         <v>43877</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" customHeight="1" spans="1:6">
-      <c r="A5" s="5" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" ht="14" customHeight="1" spans="1:6">
+      <c r="A5" s="6" t="s">
         <v>298</v>
       </c>
       <c r="B5" t="s">
@@ -5083,107 +5105,107 @@
       <c r="C5" t="s">
         <v>297</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="9">
         <v>43877</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" ht="48" customHeight="1" spans="1:6">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="9">
         <v>43867</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" ht="45" customHeight="1" spans="2:6">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="9">
         <v>43867</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" ht="44" customHeight="1" spans="1:6">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="9">
         <v>43936</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" ht="47" customHeight="1" spans="2:6">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>309</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="9">
         <v>43936</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" ht="48" customHeight="1" spans="1:6">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="9">
         <v>43876</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5206,58 +5228,58 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.73148148148148" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="62.4545454545455" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.72727272727273" style="1"/>
+    <col min="1" max="1" width="62.4537037037037" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="8.73148148148148" style="2"/>
   </cols>
   <sheetData>
     <row r="1" ht="23" customHeight="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="2" ht="42" spans="1:1">
-      <c r="A2" s="2" t="s">
+    <row r="2" ht="43.2" spans="1:1">
+      <c r="A2" s="3" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="4" ht="121" customHeight="1" spans="1:1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="3"/>
+      <c r="A8" s="4"/>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5274,10 +5296,10 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.73148148148148" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.2727272727273" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.72727272727273" style="1"/>
+    <col min="1" max="1" width="10.2685185185185" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="8.73148148148148" style="2"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5294,9 +5316,9 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="8.73148148148148" defaultRowHeight="14.4" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="124.545454545455" customWidth="1"/>
+    <col min="1" max="1" width="124.546296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -5325,13 +5347,13 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.73148148148148" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="113.636363636364" customWidth="1"/>
+    <col min="1" max="1" width="113.638888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -5343,4 +5365,51 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="16.6666666666667" customWidth="1"/>
+    <col min="2" max="2" width="18.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="20.5555555555556" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="linkknown@163.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>